<commit_message>
Mise en forme du premier tableau(bleu)
</commit_message>
<xml_diff>
--- a/ExerciceExcel4/Islam_Shafaatul_Exercice04_OpersFoncCond.xlsx
+++ b/ExerciceExcel4/Islam_Shafaatul_Exercice04_OpersFoncCond.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4fc197a25ccdc5fa/Desktop/GitHub2022/ExerceExcel4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\CVM\Outil de gestion\GitHub2022\ExerciceExcel4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="11_883F25CA4679BAF94D55383C713E0A79963B661D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC4F670C-D3E9-43DE-B4B4-3F56BB1C05A9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50FD023E-4AB8-4630-AEA8-3AFEE3F6EFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Résultats attendus" sheetId="6" r:id="rId1"/>
@@ -1342,7 +1342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection hidden="1"/>
@@ -1686,6 +1686,70 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection hidden="1"/>
@@ -1698,18 +1762,6 @@
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection hidden="1"/>
@@ -1738,14 +1790,6 @@
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -1768,38 +1812,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1814,26 +1826,6 @@
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -1842,11 +1834,31 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1872,10 +1884,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2205,191 +2213,191 @@
       <selection activeCell="AK29" sqref="AK29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.375" defaultRowHeight="10.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="16.875" style="9" customWidth="1"/>
-    <col min="5" max="6" width="11.375" style="1"/>
-    <col min="7" max="8" width="11.375" style="1" customWidth="1"/>
-    <col min="9" max="10" width="14.25" style="1" customWidth="1"/>
-    <col min="11" max="11" width="1.375" style="2" customWidth="1"/>
-    <col min="12" max="13" width="11.375" style="1" customWidth="1"/>
-    <col min="14" max="15" width="14.25" style="1" customWidth="1"/>
-    <col min="16" max="16" width="11.375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="1.375" style="15" customWidth="1"/>
-    <col min="18" max="19" width="14.25" style="1" customWidth="1"/>
-    <col min="20" max="20" width="0.875" style="15" customWidth="1"/>
-    <col min="21" max="32" width="10.75" style="1" customWidth="1"/>
-    <col min="33" max="33" width="0.875" style="15" customWidth="1"/>
-    <col min="34" max="34" width="14.25" style="1" customWidth="1"/>
-    <col min="35" max="16384" width="11.375" style="1"/>
+    <col min="1" max="1" width="1.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" style="9" customWidth="1"/>
+    <col min="5" max="6" width="11.33203125" style="1"/>
+    <col min="7" max="8" width="11.33203125" style="1" customWidth="1"/>
+    <col min="9" max="10" width="14.1640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="1.33203125" style="2" customWidth="1"/>
+    <col min="12" max="13" width="11.33203125" style="1" customWidth="1"/>
+    <col min="14" max="15" width="14.1640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="11.33203125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="1.33203125" style="15" customWidth="1"/>
+    <col min="18" max="19" width="14.1640625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="0.83203125" style="15" customWidth="1"/>
+    <col min="21" max="32" width="10.6640625" style="1" customWidth="1"/>
+    <col min="33" max="33" width="0.83203125" style="15" customWidth="1"/>
+    <col min="34" max="34" width="14.1640625" style="1" customWidth="1"/>
+    <col min="35" max="16384" width="11.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:34" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:34" ht="18.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="97" t="s">
+    <row r="1" spans="2:34" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:34" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="113" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-      <c r="O2" s="97"/>
-      <c r="P2" s="97"/>
-      <c r="Q2" s="97"/>
-      <c r="R2" s="97"/>
-      <c r="S2" s="97"/>
-      <c r="T2" s="97"/>
-      <c r="U2" s="97"/>
-      <c r="V2" s="97"/>
-      <c r="W2" s="97"/>
-      <c r="X2" s="97"/>
-      <c r="Y2" s="97"/>
-      <c r="Z2" s="97"/>
-      <c r="AA2" s="97"/>
-      <c r="AB2" s="97"/>
-      <c r="AC2" s="97"/>
-      <c r="AD2" s="97"/>
-      <c r="AE2" s="97"/>
-      <c r="AF2" s="97"/>
-      <c r="AG2" s="97"/>
-      <c r="AH2" s="97"/>
-    </row>
-    <row r="3" spans="2:34" ht="11" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="113"/>
+      <c r="H2" s="113"/>
+      <c r="I2" s="113"/>
+      <c r="J2" s="113"/>
+      <c r="K2" s="113"/>
+      <c r="L2" s="113"/>
+      <c r="M2" s="113"/>
+      <c r="N2" s="113"/>
+      <c r="O2" s="113"/>
+      <c r="P2" s="113"/>
+      <c r="Q2" s="113"/>
+      <c r="R2" s="113"/>
+      <c r="S2" s="113"/>
+      <c r="T2" s="113"/>
+      <c r="U2" s="113"/>
+      <c r="V2" s="113"/>
+      <c r="W2" s="113"/>
+      <c r="X2" s="113"/>
+      <c r="Y2" s="113"/>
+      <c r="Z2" s="113"/>
+      <c r="AA2" s="113"/>
+      <c r="AB2" s="113"/>
+      <c r="AC2" s="113"/>
+      <c r="AD2" s="113"/>
+      <c r="AE2" s="113"/>
+      <c r="AF2" s="113"/>
+      <c r="AG2" s="113"/>
+      <c r="AH2" s="113"/>
+    </row>
+    <row r="3" spans="2:34" ht="12" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
     </row>
-    <row r="4" spans="2:34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:34" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="98" t="s">
+    <row r="4" spans="2:34" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="2:34" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="114" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="98"/>
-      <c r="D5" s="98"/>
-      <c r="E5" s="98"/>
-      <c r="F5" s="98"/>
-      <c r="G5" s="98"/>
-      <c r="H5" s="98"/>
-      <c r="I5" s="98"/>
-      <c r="J5" s="98"/>
-      <c r="L5" s="99" t="s">
+      <c r="C5" s="114"/>
+      <c r="D5" s="114"/>
+      <c r="E5" s="114"/>
+      <c r="F5" s="114"/>
+      <c r="G5" s="114"/>
+      <c r="H5" s="114"/>
+      <c r="I5" s="114"/>
+      <c r="J5" s="114"/>
+      <c r="L5" s="115" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="99"/>
-      <c r="N5" s="99"/>
-      <c r="O5" s="99"/>
-      <c r="P5" s="99"/>
-      <c r="R5" s="103" t="s">
+      <c r="M5" s="115"/>
+      <c r="N5" s="115"/>
+      <c r="O5" s="115"/>
+      <c r="P5" s="115"/>
+      <c r="R5" s="116" t="s">
         <v>11</v>
       </c>
-      <c r="S5" s="103"/>
-      <c r="T5" s="103"/>
-      <c r="U5" s="103"/>
-      <c r="V5" s="103"/>
-      <c r="W5" s="103"/>
-      <c r="X5" s="103"/>
-      <c r="Y5" s="103"/>
-      <c r="Z5" s="103"/>
-      <c r="AA5" s="103"/>
-      <c r="AB5" s="103"/>
-      <c r="AC5" s="103"/>
-      <c r="AD5" s="103"/>
-      <c r="AE5" s="103"/>
-      <c r="AF5" s="103"/>
-      <c r="AG5" s="103"/>
-      <c r="AH5" s="103"/>
-    </row>
-    <row r="6" spans="2:34" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="120" t="s">
+      <c r="S5" s="116"/>
+      <c r="T5" s="116"/>
+      <c r="U5" s="116"/>
+      <c r="V5" s="116"/>
+      <c r="W5" s="116"/>
+      <c r="X5" s="116"/>
+      <c r="Y5" s="116"/>
+      <c r="Z5" s="116"/>
+      <c r="AA5" s="116"/>
+      <c r="AB5" s="116"/>
+      <c r="AC5" s="116"/>
+      <c r="AD5" s="116"/>
+      <c r="AE5" s="116"/>
+      <c r="AF5" s="116"/>
+      <c r="AG5" s="116"/>
+      <c r="AH5" s="116"/>
+    </row>
+    <row r="6" spans="2:34" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="112" t="s">
+      <c r="C7" s="123" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="114" t="s">
+      <c r="D7" s="125" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="104" t="s">
+      <c r="E7" s="117" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="116" t="s">
+      <c r="F7" s="127" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="106" t="s">
+      <c r="G7" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="107"/>
-      <c r="I7" s="118" t="s">
+      <c r="H7" s="120"/>
+      <c r="I7" s="100" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="119"/>
+      <c r="J7" s="101"/>
       <c r="K7" s="4"/>
-      <c r="L7" s="108" t="s">
+      <c r="L7" s="121" t="s">
         <v>2</v>
       </c>
-      <c r="M7" s="109"/>
-      <c r="N7" s="108" t="s">
-        <v>0</v>
-      </c>
-      <c r="O7" s="109"/>
-      <c r="P7" s="122" t="s">
+      <c r="M7" s="122"/>
+      <c r="N7" s="121" t="s">
+        <v>0</v>
+      </c>
+      <c r="O7" s="122"/>
+      <c r="P7" s="109" t="s">
         <v>42</v>
       </c>
       <c r="Q7" s="17"/>
-      <c r="R7" s="110" t="s">
+      <c r="R7" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="S7" s="111"/>
+      <c r="S7" s="103"/>
       <c r="T7" s="13"/>
-      <c r="U7" s="110" t="s">
+      <c r="U7" s="102" t="s">
         <v>38</v>
       </c>
-      <c r="V7" s="111"/>
-      <c r="W7" s="110" t="s">
+      <c r="V7" s="103"/>
+      <c r="W7" s="102" t="s">
         <v>41</v>
       </c>
-      <c r="X7" s="111"/>
-      <c r="Y7" s="110" t="s">
+      <c r="X7" s="103"/>
+      <c r="Y7" s="102" t="s">
         <v>43</v>
       </c>
-      <c r="Z7" s="111"/>
-      <c r="AA7" s="110" t="s">
+      <c r="Z7" s="103"/>
+      <c r="AA7" s="102" t="s">
         <v>44</v>
       </c>
-      <c r="AB7" s="111"/>
-      <c r="AC7" s="110" t="s">
+      <c r="AB7" s="103"/>
+      <c r="AC7" s="102" t="s">
         <v>45</v>
       </c>
-      <c r="AD7" s="111"/>
-      <c r="AE7" s="110" t="s">
+      <c r="AD7" s="103"/>
+      <c r="AE7" s="102" t="s">
         <v>46</v>
       </c>
-      <c r="AF7" s="111"/>
+      <c r="AF7" s="103"/>
       <c r="AG7" s="13"/>
-      <c r="AH7" s="124" t="s">
+      <c r="AH7" s="111" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="2:34" ht="10.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="121"/>
-      <c r="C8" s="113"/>
-      <c r="D8" s="115"/>
-      <c r="E8" s="105"/>
-      <c r="F8" s="117"/>
+    <row r="8" spans="2:34" ht="10.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="108"/>
+      <c r="C8" s="124"/>
+      <c r="D8" s="126"/>
+      <c r="E8" s="118"/>
+      <c r="F8" s="128"/>
       <c r="G8" s="18" t="s">
         <v>9</v>
       </c>
@@ -2415,7 +2423,7 @@
       <c r="O8" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="P8" s="123"/>
+      <c r="P8" s="110"/>
       <c r="Q8" s="17"/>
       <c r="R8" s="25" t="s">
         <v>9</v>
@@ -2461,9 +2469,9 @@
         <v>40</v>
       </c>
       <c r="AG8" s="16"/>
-      <c r="AH8" s="125"/>
-    </row>
-    <row r="9" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH8" s="112"/>
+    </row>
+    <row r="9" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="44" t="s">
         <v>15</v>
       </c>
@@ -2574,7 +2582,7 @@
         <v>44123.068559822648</v>
       </c>
     </row>
-    <row r="10" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="52" t="s">
         <v>16</v>
       </c>
@@ -2685,7 +2693,7 @@
         <v>46803.39935</v>
       </c>
     </row>
-    <row r="11" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="58" t="s">
         <v>17</v>
       </c>
@@ -2796,7 +2804,7 @@
         <v>53460.689941820616</v>
       </c>
     </row>
-    <row r="12" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="52" t="s">
         <v>18</v>
       </c>
@@ -2907,7 +2915,7 @@
         <v>56091.271043346751</v>
       </c>
     </row>
-    <row r="13" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="58" t="s">
         <v>19</v>
       </c>
@@ -3018,7 +3026,7 @@
         <v>66132.912698011307</v>
       </c>
     </row>
-    <row r="14" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="52" t="s">
         <v>20</v>
       </c>
@@ -3129,7 +3137,7 @@
         <v>47649.283900000002</v>
       </c>
     </row>
-    <row r="15" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="58" t="s">
         <v>21</v>
       </c>
@@ -3240,7 +3248,7 @@
         <v>63645.095529451653</v>
       </c>
     </row>
-    <row r="16" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="52" t="s">
         <v>22</v>
       </c>
@@ -3351,7 +3359,7 @@
         <v>59316.886749999991</v>
       </c>
     </row>
-    <row r="17" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="58" t="s">
         <v>23</v>
       </c>
@@ -3462,7 +3470,7 @@
         <v>50963.016009185478</v>
       </c>
     </row>
-    <row r="18" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="52" t="s">
         <v>24</v>
       </c>
@@ -3573,7 +3581,7 @@
         <v>76982.1446</v>
       </c>
     </row>
-    <row r="19" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="58" t="s">
         <v>25</v>
       </c>
@@ -3684,7 +3692,7 @@
         <v>30746.00995</v>
       </c>
     </row>
-    <row r="20" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="52" t="s">
         <v>26</v>
       </c>
@@ -3795,7 +3803,7 @@
         <v>73562.36914414019</v>
       </c>
     </row>
-    <row r="21" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="58" t="s">
         <v>27</v>
       </c>
@@ -3906,7 +3914,7 @@
         <v>49994.442049999998</v>
       </c>
     </row>
-    <row r="22" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="52" t="s">
         <v>28</v>
       </c>
@@ -4017,7 +4025,7 @@
         <v>69812.4228</v>
       </c>
     </row>
-    <row r="23" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="58" t="s">
         <v>29</v>
       </c>
@@ -4128,7 +4136,7 @@
         <v>37807.700653177162</v>
       </c>
     </row>
-    <row r="24" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="20" t="s">
         <v>30</v>
       </c>
@@ -4239,7 +4247,7 @@
         <v>73799.865699999995</v>
       </c>
     </row>
-    <row r="25" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="21" t="s">
         <v>31</v>
       </c>
@@ -4350,7 +4358,7 @@
         <v>81369.813249999992</v>
       </c>
     </row>
-    <row r="26" spans="2:34" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:34" ht="3" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R26" s="36"/>
       <c r="S26" s="36"/>
       <c r="T26" s="37"/>
@@ -4369,7 +4377,7 @@
       <c r="AG26" s="37"/>
       <c r="AH26" s="36"/>
     </row>
-    <row r="27" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I27" s="66">
         <f t="shared" ref="I27:J27" si="17">SUM(I9:I26)</f>
         <v>1508346.0400000003</v>
@@ -4436,7 +4444,7 @@
         <v>982260.3919289558</v>
       </c>
     </row>
-    <row r="28" spans="2:34" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:34" ht="3" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
@@ -4464,57 +4472,57 @@
       <c r="AG28" s="14"/>
       <c r="AH28" s="5"/>
     </row>
-    <row r="29" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="B29" s="100" t="s">
+    <row r="29" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="B29" s="104" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="101"/>
-      <c r="D29" s="102"/>
-      <c r="E29" s="100" t="s">
+      <c r="C29" s="105"/>
+      <c r="D29" s="106"/>
+      <c r="E29" s="104" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="102"/>
-      <c r="G29" s="100" t="s">
+      <c r="F29" s="106"/>
+      <c r="G29" s="104" t="s">
         <v>12</v>
       </c>
-      <c r="H29" s="101"/>
-      <c r="I29" s="101"/>
-      <c r="J29" s="101"/>
-      <c r="K29" s="101"/>
-      <c r="L29" s="101"/>
-      <c r="M29" s="101"/>
-      <c r="N29" s="101"/>
-      <c r="O29" s="101"/>
-      <c r="P29" s="102"/>
-      <c r="R29" s="100" t="s">
+      <c r="H29" s="105"/>
+      <c r="I29" s="105"/>
+      <c r="J29" s="105"/>
+      <c r="K29" s="105"/>
+      <c r="L29" s="105"/>
+      <c r="M29" s="105"/>
+      <c r="N29" s="105"/>
+      <c r="O29" s="105"/>
+      <c r="P29" s="106"/>
+      <c r="R29" s="104" t="s">
         <v>13</v>
       </c>
-      <c r="S29" s="101"/>
-      <c r="T29" s="101"/>
-      <c r="U29" s="101"/>
-      <c r="V29" s="101"/>
-      <c r="W29" s="101"/>
-      <c r="X29" s="101"/>
-      <c r="Y29" s="101"/>
-      <c r="Z29" s="101"/>
-      <c r="AA29" s="101"/>
-      <c r="AB29" s="101"/>
-      <c r="AC29" s="101"/>
-      <c r="AD29" s="101"/>
-      <c r="AE29" s="101"/>
-      <c r="AF29" s="101"/>
-      <c r="AG29" s="101"/>
-      <c r="AH29" s="102"/>
-    </row>
-    <row r="31" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="S29" s="105"/>
+      <c r="T29" s="105"/>
+      <c r="U29" s="105"/>
+      <c r="V29" s="105"/>
+      <c r="W29" s="105"/>
+      <c r="X29" s="105"/>
+      <c r="Y29" s="105"/>
+      <c r="Z29" s="105"/>
+      <c r="AA29" s="105"/>
+      <c r="AB29" s="105"/>
+      <c r="AC29" s="105"/>
+      <c r="AD29" s="105"/>
+      <c r="AE29" s="105"/>
+      <c r="AF29" s="105"/>
+      <c r="AG29" s="105"/>
+      <c r="AH29" s="106"/>
+    </row>
+    <row r="31" spans="2:34" x14ac:dyDescent="0.2">
       <c r="E31" s="10"/>
     </row>
-    <row r="32" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:34" x14ac:dyDescent="0.2">
       <c r="D32" s="11"/>
       <c r="L32" s="12"/>
       <c r="R32" s="5"/>
     </row>
-    <row r="33" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:33" x14ac:dyDescent="0.2">
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
@@ -4525,7 +4533,7 @@
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
     </row>
-    <row r="34" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:33" x14ac:dyDescent="0.2">
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="G34" s="5"/>
@@ -4541,7 +4549,7 @@
       <c r="T34" s="1"/>
       <c r="AG34" s="1"/>
     </row>
-    <row r="35" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:33" x14ac:dyDescent="0.2">
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="G35" s="5"/>
@@ -4557,7 +4565,7 @@
       <c r="T35" s="1"/>
       <c r="AG35" s="1"/>
     </row>
-    <row r="36" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:33" x14ac:dyDescent="0.2">
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="G36" s="5"/>
@@ -4573,7 +4581,7 @@
       <c r="T36" s="1"/>
       <c r="AG36" s="1"/>
     </row>
-    <row r="37" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:33" x14ac:dyDescent="0.2">
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="G37" s="5"/>
@@ -4589,7 +4597,7 @@
       <c r="T37" s="1"/>
       <c r="AG37" s="1"/>
     </row>
-    <row r="38" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:33" x14ac:dyDescent="0.2">
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="G38" s="5"/>
@@ -4605,7 +4613,7 @@
       <c r="T38" s="1"/>
       <c r="AG38" s="1"/>
     </row>
-    <row r="39" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:33" x14ac:dyDescent="0.2">
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="G39" s="5"/>
@@ -4621,7 +4629,7 @@
       <c r="T39" s="1"/>
       <c r="AG39" s="1"/>
     </row>
-    <row r="40" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:33" x14ac:dyDescent="0.2">
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="G40" s="5"/>
@@ -4637,7 +4645,7 @@
       <c r="T40" s="1"/>
       <c r="AG40" s="1"/>
     </row>
-    <row r="41" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:33" x14ac:dyDescent="0.2">
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="G41" s="5"/>
@@ -4653,7 +4661,7 @@
       <c r="T41" s="1"/>
       <c r="AG41" s="1"/>
     </row>
-    <row r="42" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:33" x14ac:dyDescent="0.2">
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="G42" s="5"/>
@@ -4669,7 +4677,7 @@
       <c r="T42" s="1"/>
       <c r="AG42" s="1"/>
     </row>
-    <row r="43" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:33" x14ac:dyDescent="0.2">
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="G43" s="5"/>
@@ -4685,7 +4693,7 @@
       <c r="T43" s="1"/>
       <c r="AG43" s="1"/>
     </row>
-    <row r="44" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:33" x14ac:dyDescent="0.2">
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="G44" s="5"/>
@@ -4701,7 +4709,7 @@
       <c r="T44" s="1"/>
       <c r="AG44" s="1"/>
     </row>
-    <row r="45" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:33" x14ac:dyDescent="0.2">
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="G45" s="5"/>
@@ -4717,7 +4725,7 @@
       <c r="T45" s="1"/>
       <c r="AG45" s="1"/>
     </row>
-    <row r="46" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:33" x14ac:dyDescent="0.2">
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="G46" s="5"/>
@@ -4733,7 +4741,7 @@
       <c r="T46" s="1"/>
       <c r="AG46" s="1"/>
     </row>
-    <row r="47" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:33" x14ac:dyDescent="0.2">
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="G47" s="5"/>
@@ -4749,7 +4757,7 @@
       <c r="T47" s="1"/>
       <c r="AG47" s="1"/>
     </row>
-    <row r="48" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:33" x14ac:dyDescent="0.2">
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="G48" s="5"/>
@@ -4765,7 +4773,7 @@
       <c r="T48" s="1"/>
       <c r="AG48" s="1"/>
     </row>
-    <row r="49" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:33" x14ac:dyDescent="0.2">
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="G49" s="5"/>
@@ -4781,7 +4789,7 @@
       <c r="T49" s="1"/>
       <c r="AG49" s="1"/>
     </row>
-    <row r="50" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:33" x14ac:dyDescent="0.2">
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="G50" s="5"/>
@@ -4797,7 +4805,7 @@
       <c r="T50" s="1"/>
       <c r="AG50" s="1"/>
     </row>
-    <row r="51" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:33" x14ac:dyDescent="0.2">
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="G51" s="5"/>
@@ -4813,7 +4821,7 @@
       <c r="T51" s="1"/>
       <c r="AG51" s="1"/>
     </row>
-    <row r="52" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:33" x14ac:dyDescent="0.2">
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="G52" s="5"/>
@@ -4829,7 +4837,7 @@
       <c r="T52" s="1"/>
       <c r="AG52" s="1"/>
     </row>
-    <row r="53" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:33" x14ac:dyDescent="0.2">
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="G53" s="5"/>
@@ -4845,7 +4853,7 @@
       <c r="T53" s="1"/>
       <c r="AG53" s="1"/>
     </row>
-    <row r="54" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:33" x14ac:dyDescent="0.2">
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="G54" s="5"/>
@@ -4861,7 +4869,7 @@
       <c r="T54" s="1"/>
       <c r="AG54" s="1"/>
     </row>
-    <row r="55" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:33" x14ac:dyDescent="0.2">
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="G55" s="5"/>
@@ -4883,16 +4891,6 @@
     <sortCondition ref="AL9"/>
   </sortState>
   <mergeCells count="26">
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="W7:X7"/>
-    <mergeCell ref="R29:AH29"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="Y7:Z7"/>
-    <mergeCell ref="AA7:AB7"/>
-    <mergeCell ref="AC7:AD7"/>
-    <mergeCell ref="AE7:AF7"/>
-    <mergeCell ref="AH7:AH8"/>
     <mergeCell ref="B2:AH2"/>
     <mergeCell ref="B5:J5"/>
     <mergeCell ref="L5:P5"/>
@@ -4909,6 +4907,16 @@
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="U7:V7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="W7:X7"/>
+    <mergeCell ref="R29:AH29"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="Y7:Z7"/>
+    <mergeCell ref="AA7:AB7"/>
+    <mergeCell ref="AC7:AD7"/>
+    <mergeCell ref="AE7:AF7"/>
+    <mergeCell ref="AH7:AH8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="125" orientation="portrait" r:id="rId1"/>
@@ -4924,23 +4932,23 @@
   <dimension ref="B2:AH33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.75" defaultRowHeight="10.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.75" style="92"/>
+    <col min="1" max="1" width="10.6640625" style="92"/>
     <col min="2" max="2" width="31.5" style="92" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.75" style="92"/>
-    <col min="4" max="4" width="16.75" style="92" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="92"/>
+    <col min="4" max="4" width="16.6640625" style="92" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" style="92" customWidth="1"/>
-    <col min="6" max="8" width="10.75" style="92"/>
-    <col min="9" max="9" width="14.625" style="92" customWidth="1"/>
-    <col min="10" max="10" width="10.625" style="92" customWidth="1"/>
-    <col min="11" max="16384" width="10.75" style="92"/>
+    <col min="6" max="8" width="10.6640625" style="92"/>
+    <col min="9" max="9" width="14.6640625" style="92" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" style="92" customWidth="1"/>
+    <col min="11" max="16384" width="10.6640625" style="92"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:34" ht="20.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:34" ht="20.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="94" t="s">
         <v>14</v>
       </c>
@@ -4977,76 +4985,76 @@
       <c r="AG2" s="95"/>
       <c r="AH2" s="95"/>
     </row>
-    <row r="3" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="96" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="126" t="s">
+    <row r="4" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="129" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="126"/>
-      <c r="D5" s="126"/>
-      <c r="E5" s="126"/>
-      <c r="F5" s="126"/>
-      <c r="G5" s="126"/>
-      <c r="H5" s="126"/>
-      <c r="I5" s="126"/>
-      <c r="J5" s="126"/>
-      <c r="L5" s="127" t="s">
+      <c r="C5" s="129"/>
+      <c r="D5" s="129"/>
+      <c r="E5" s="129"/>
+      <c r="F5" s="129"/>
+      <c r="G5" s="129"/>
+      <c r="H5" s="129"/>
+      <c r="I5" s="129"/>
+      <c r="J5" s="129"/>
+      <c r="L5" s="130" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="127"/>
-      <c r="N5" s="127"/>
-      <c r="O5" s="127"/>
-      <c r="P5" s="127"/>
-      <c r="R5" s="128" t="s">
+      <c r="M5" s="130"/>
+      <c r="N5" s="130"/>
+      <c r="O5" s="130"/>
+      <c r="P5" s="130"/>
+      <c r="R5" s="131" t="s">
         <v>11</v>
       </c>
-      <c r="S5" s="128"/>
-      <c r="T5" s="128"/>
-      <c r="U5" s="128"/>
-      <c r="V5" s="128"/>
-      <c r="W5" s="128"/>
-      <c r="X5" s="128"/>
-      <c r="Y5" s="128"/>
-      <c r="Z5" s="128"/>
-      <c r="AA5" s="128"/>
-      <c r="AB5" s="128"/>
-      <c r="AC5" s="128"/>
-      <c r="AD5" s="128"/>
-      <c r="AE5" s="128"/>
-      <c r="AF5" s="128"/>
-      <c r="AG5" s="128"/>
-      <c r="AH5" s="128"/>
-    </row>
-    <row r="6" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="134" t="s">
+      <c r="S5" s="131"/>
+      <c r="T5" s="131"/>
+      <c r="U5" s="131"/>
+      <c r="V5" s="131"/>
+      <c r="W5" s="131"/>
+      <c r="X5" s="131"/>
+      <c r="Y5" s="131"/>
+      <c r="Z5" s="131"/>
+      <c r="AA5" s="131"/>
+      <c r="AB5" s="131"/>
+      <c r="AC5" s="131"/>
+      <c r="AD5" s="131"/>
+      <c r="AE5" s="131"/>
+      <c r="AF5" s="131"/>
+      <c r="AG5" s="131"/>
+      <c r="AH5" s="131"/>
+    </row>
+    <row r="6" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="134" t="s">
+      <c r="C7" s="132" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="134" t="s">
+      <c r="D7" s="132" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="135" t="s">
+      <c r="E7" s="133" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="135" t="s">
+      <c r="F7" s="133" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="134" t="s">
+      <c r="G7" s="132" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="134"/>
-      <c r="I7" s="134" t="s">
+      <c r="H7" s="132"/>
+      <c r="I7" s="132" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="134"/>
+      <c r="J7" s="132"/>
       <c r="L7" s="92" t="s">
         <v>2</v>
       </c>
@@ -5081,22 +5089,22 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="134"/>
-      <c r="C8" s="134"/>
-      <c r="D8" s="134"/>
-      <c r="E8" s="135"/>
-      <c r="F8" s="135"/>
-      <c r="G8" s="133" t="s">
+    <row r="8" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="132"/>
+      <c r="C8" s="132"/>
+      <c r="D8" s="132"/>
+      <c r="E8" s="133"/>
+      <c r="F8" s="133"/>
+      <c r="G8" s="97" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="133" t="s">
+      <c r="H8" s="97" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="133" t="s">
+      <c r="I8" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="J8" s="133" t="s">
+      <c r="J8" s="97" t="s">
         <v>4</v>
       </c>
       <c r="L8" s="92" t="s">
@@ -5114,17 +5122,17 @@
       <c r="P8" s="93"/>
       <c r="AH8" s="93"/>
     </row>
-    <row r="9" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="93" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="136">
+      <c r="D9" s="98">
         <v>38226</v>
       </c>
-      <c r="E9" s="137" t="s">
+      <c r="E9" s="99" t="s">
         <v>69</v>
       </c>
       <c r="G9" s="92">
@@ -5158,26 +5166,28 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="93" t="s">
+    <row r="10" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="138" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="93" t="s">
+      <c r="C10" s="138" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="136">
+      <c r="D10" s="139">
         <v>37601</v>
       </c>
-      <c r="G10" s="92">
+      <c r="E10" s="140"/>
+      <c r="F10" s="140"/>
+      <c r="G10" s="140">
         <v>23.05</v>
       </c>
-      <c r="H10" s="92">
+      <c r="H10" s="140">
         <v>34.58</v>
       </c>
-      <c r="I10" s="92">
+      <c r="I10" s="140">
         <v>86104.49</v>
       </c>
-      <c r="J10" s="92">
+      <c r="J10" s="140">
         <v>141119.44</v>
       </c>
       <c r="K10" s="92">
@@ -5199,14 +5209,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="93" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="93" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="136">
+      <c r="D11" s="98">
         <v>35826</v>
       </c>
       <c r="G11" s="92">
@@ -5240,26 +5250,28 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="93" t="s">
+    <row r="12" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="138" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="93" t="s">
+      <c r="C12" s="138" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="136">
+      <c r="D12" s="139">
         <v>35403</v>
       </c>
-      <c r="G12" s="92">
+      <c r="E12" s="140"/>
+      <c r="F12" s="140"/>
+      <c r="G12" s="140">
         <v>27.87</v>
       </c>
-      <c r="H12" s="92">
+      <c r="H12" s="140">
         <v>41.81</v>
       </c>
-      <c r="I12" s="92">
+      <c r="I12" s="140">
         <v>88556.09</v>
       </c>
-      <c r="J12" s="92">
+      <c r="J12" s="140">
         <v>156576.41</v>
       </c>
       <c r="K12" s="92">
@@ -5281,14 +5293,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="93" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="93" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="136">
+      <c r="D13" s="98">
         <v>33093</v>
       </c>
       <c r="G13" s="92">
@@ -5322,26 +5334,28 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="93" t="s">
+    <row r="14" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="138" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="93" t="s">
+      <c r="C14" s="138" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="136">
+      <c r="D14" s="139">
         <v>37900</v>
       </c>
-      <c r="G14" s="92">
+      <c r="E14" s="140"/>
+      <c r="F14" s="140"/>
+      <c r="G14" s="140">
         <v>22.4</v>
       </c>
-      <c r="H14" s="92">
+      <c r="H14" s="140">
         <v>33.6</v>
       </c>
-      <c r="I14" s="92">
+      <c r="I14" s="140">
         <v>87296.23</v>
       </c>
-      <c r="J14" s="92">
+      <c r="J14" s="140">
         <v>141450.34</v>
       </c>
       <c r="K14" s="92">
@@ -5363,14 +5377,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="93" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="136">
+      <c r="D15" s="98">
         <v>35590</v>
       </c>
       <c r="G15" s="92">
@@ -5404,26 +5418,28 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="2:34" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="93" t="s">
+    <row r="16" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="138" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="93" t="s">
+      <c r="C16" s="138" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="136">
+      <c r="D16" s="139">
         <v>35192</v>
       </c>
-      <c r="G16" s="92">
+      <c r="E16" s="140"/>
+      <c r="F16" s="140"/>
+      <c r="G16" s="140">
         <v>28.33</v>
       </c>
-      <c r="H16" s="92">
+      <c r="H16" s="140">
         <v>42.5</v>
       </c>
-      <c r="I16" s="92">
+      <c r="I16" s="140">
         <v>88963.64</v>
       </c>
-      <c r="J16" s="92">
+      <c r="J16" s="140">
         <v>158342.45000000001</v>
       </c>
       <c r="K16" s="92">
@@ -5445,14 +5461,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:18" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:18" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="93" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="136">
+      <c r="D17" s="98">
         <v>36628</v>
       </c>
       <c r="G17" s="92">
@@ -5486,26 +5502,28 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="2:18" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="93" t="s">
+    <row r="18" spans="2:18" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="138" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="93" t="s">
+      <c r="C18" s="138" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="136">
+      <c r="D18" s="139">
         <v>30115</v>
       </c>
-      <c r="G18" s="92">
+      <c r="E18" s="140"/>
+      <c r="F18" s="140"/>
+      <c r="G18" s="140">
         <v>39.46</v>
       </c>
-      <c r="H18" s="92">
+      <c r="H18" s="140">
         <v>59.19</v>
       </c>
-      <c r="I18" s="92">
+      <c r="I18" s="140">
         <v>92465.44</v>
       </c>
-      <c r="J18" s="92">
+      <c r="J18" s="140">
         <v>188016.91</v>
       </c>
       <c r="K18" s="92">
@@ -5527,14 +5545,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="2:18" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:18" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="93" t="s">
         <v>25</v>
       </c>
       <c r="C19" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="136">
+      <c r="D19" s="98">
         <v>41231</v>
       </c>
       <c r="G19" s="92">
@@ -5568,26 +5586,28 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="2:18" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="93" t="s">
+    <row r="20" spans="2:18" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="138" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="93" t="s">
+      <c r="C20" s="138" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="136">
+      <c r="D20" s="139">
         <v>31824</v>
       </c>
-      <c r="G20" s="92">
+      <c r="E20" s="140"/>
+      <c r="F20" s="140"/>
+      <c r="G20" s="140">
         <v>35.71</v>
       </c>
-      <c r="H20" s="92">
+      <c r="H20" s="140">
         <v>53.57</v>
       </c>
-      <c r="I20" s="92">
+      <c r="I20" s="140">
         <v>91406.45</v>
       </c>
-      <c r="J20" s="92">
+      <c r="J20" s="140">
         <v>178594.61</v>
       </c>
       <c r="K20" s="92">
@@ -5609,14 +5629,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="2:18" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:18" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="93" t="s">
         <v>27</v>
       </c>
       <c r="C21" s="93" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="136">
+      <c r="D21" s="98">
         <v>38150</v>
       </c>
       <c r="G21" s="92">
@@ -5650,26 +5670,28 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:18" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="93" t="s">
+    <row r="22" spans="2:18" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="138" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="93" t="s">
+      <c r="C22" s="138" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="136">
+      <c r="D22" s="139">
         <v>32891</v>
       </c>
-      <c r="G22" s="92">
+      <c r="E22" s="140"/>
+      <c r="F22" s="140"/>
+      <c r="G22" s="140">
         <v>33.380000000000003</v>
       </c>
-      <c r="H22" s="92">
+      <c r="H22" s="140">
         <v>50.06</v>
       </c>
-      <c r="I22" s="92">
+      <c r="I22" s="140">
         <v>91420.63</v>
       </c>
-      <c r="J22" s="92">
+      <c r="J22" s="140">
         <v>173822.75</v>
       </c>
       <c r="K22" s="92">
@@ -5691,14 +5713,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="2:18" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:18" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="93" t="s">
         <v>29</v>
       </c>
       <c r="C23" s="93" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="136">
+      <c r="D23" s="98">
         <v>41102</v>
       </c>
       <c r="G23" s="92">
@@ -5732,26 +5754,28 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="2:18" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="92" t="s">
+    <row r="24" spans="2:18" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="140" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="92" t="s">
+      <c r="C24" s="140" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="136">
+      <c r="D24" s="139">
         <v>29465</v>
       </c>
-      <c r="G24" s="92">
+      <c r="E24" s="140"/>
+      <c r="F24" s="140"/>
+      <c r="G24" s="140">
         <v>40.880000000000003</v>
       </c>
-      <c r="H24" s="92">
+      <c r="H24" s="140">
         <v>61.33</v>
       </c>
-      <c r="I24" s="92">
+      <c r="I24" s="140">
         <v>93640.78</v>
       </c>
-      <c r="J24" s="92">
+      <c r="J24" s="140">
         <v>193110.06</v>
       </c>
       <c r="K24" s="92">
@@ -5773,14 +5797,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:18" ht="10.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:18" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="92" t="s">
         <v>31</v>
       </c>
       <c r="C25" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="136">
+      <c r="D25" s="98">
         <v>30711</v>
       </c>
       <c r="G25" s="92">
@@ -5814,10 +5838,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="2:18" ht="10.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:18" ht="10.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:18" ht="10.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:18" ht="10.35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="2:18" ht="10.35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="2:18" ht="10.35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B29" s="92" t="s">
         <v>12</v>
       </c>
@@ -5831,10 +5855,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="2:18" ht="10.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:18" ht="10.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:18" ht="10.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="10.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:18" ht="10.35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="2:18" ht="10.35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="2:18" ht="10.35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="10.35" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="B5:J5"/>
@@ -5861,61 +5885,61 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.75" defaultRowHeight="10.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.125" style="69" customWidth="1"/>
-    <col min="2" max="2" width="3.625" style="69" customWidth="1"/>
-    <col min="3" max="3" width="42.875" style="69" customWidth="1"/>
-    <col min="4" max="4" width="128.625" style="69" customWidth="1"/>
-    <col min="5" max="5" width="2.125" style="69" customWidth="1"/>
-    <col min="6" max="16384" width="11.75" style="69"/>
+    <col min="1" max="1" width="2.1640625" style="69" customWidth="1"/>
+    <col min="2" max="2" width="3.6640625" style="69" customWidth="1"/>
+    <col min="3" max="3" width="42.83203125" style="69" customWidth="1"/>
+    <col min="4" max="4" width="128.6640625" style="69" customWidth="1"/>
+    <col min="5" max="5" width="2.1640625" style="69" customWidth="1"/>
+    <col min="6" max="16384" width="11.6640625" style="69"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:4" ht="13" x14ac:dyDescent="0.25">
-      <c r="B2" s="129" t="s">
+    <row r="1" spans="2:4" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B2" s="134" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="129"/>
-      <c r="D2" s="129"/>
-    </row>
-    <row r="3" spans="2:4" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="130" t="s">
+      <c r="C2" s="134"/>
+      <c r="D2" s="134"/>
+    </row>
+    <row r="3" spans="2:4" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C4" s="135" t="s">
         <v>59</v>
       </c>
       <c r="D4" s="88" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="131"/>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C5" s="136"/>
       <c r="D5" s="70" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="131"/>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C6" s="136"/>
       <c r="D6" s="71" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="131"/>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C7" s="136"/>
       <c r="D7" s="70" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="11" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="132"/>
+    <row r="8" spans="2:4" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="137"/>
       <c r="D8" s="89" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C9" s="72"/>
     </row>
-    <row r="10" spans="2:4" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C10" s="90" t="s">
         <v>67</v>
       </c>
@@ -5923,55 +5947,55 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C11" s="72"/>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="130" t="s">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C12" s="135" t="s">
         <v>57</v>
       </c>
       <c r="D12" s="88" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C13" s="131"/>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C13" s="136"/>
       <c r="D13" s="70" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C14" s="131"/>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C14" s="136"/>
       <c r="D14" s="68" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C15" s="131"/>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C15" s="136"/>
       <c r="D15" s="87" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C16" s="131"/>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C16" s="136"/>
       <c r="D16" s="68" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" s="131"/>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C17" s="136"/>
       <c r="D17" s="87" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C18" s="131"/>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C18" s="136"/>
       <c r="D18" s="68" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="3:4" ht="11" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="132"/>
+    <row r="19" spans="3:4" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="137"/>
       <c r="D19" s="89" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Encadrement du premier tableau
</commit_message>
<xml_diff>
--- a/ExerciceExcel4/Islam_Shafaatul_Exercice04_OpersFoncCond.xlsx
+++ b/ExerciceExcel4/Islam_Shafaatul_Exercice04_OpersFoncCond.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\CVM\Outil de gestion\GitHub2022\ExerciceExcel4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50FD023E-4AB8-4630-AEA8-3AFEE3F6EFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3FB125-69E7-4E34-8D7F-8B0277FF6143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Résultats attendus" sheetId="6" r:id="rId1"/>
@@ -773,7 +773,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -870,8 +870,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="42">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -1338,11 +1344,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="3"/>
+      </left>
+      <right style="medium">
+        <color theme="3"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="3"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="3"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection hidden="1"/>
@@ -1670,26 +1705,6 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1698,6 +1713,98 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
@@ -1706,26 +1813,6 @@
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -1748,70 +1835,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1850,16 +1873,80 @@
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -2237,41 +2324,41 @@
   <sheetData>
     <row r="1" spans="2:34" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:34" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="113" t="s">
+      <c r="B2" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="113"/>
-      <c r="J2" s="113"/>
-      <c r="K2" s="113"/>
-      <c r="L2" s="113"/>
-      <c r="M2" s="113"/>
-      <c r="N2" s="113"/>
-      <c r="O2" s="113"/>
-      <c r="P2" s="113"/>
-      <c r="Q2" s="113"/>
-      <c r="R2" s="113"/>
-      <c r="S2" s="113"/>
-      <c r="T2" s="113"/>
-      <c r="U2" s="113"/>
-      <c r="V2" s="113"/>
-      <c r="W2" s="113"/>
-      <c r="X2" s="113"/>
-      <c r="Y2" s="113"/>
-      <c r="Z2" s="113"/>
-      <c r="AA2" s="113"/>
-      <c r="AB2" s="113"/>
-      <c r="AC2" s="113"/>
-      <c r="AD2" s="113"/>
-      <c r="AE2" s="113"/>
-      <c r="AF2" s="113"/>
-      <c r="AG2" s="113"/>
-      <c r="AH2" s="113"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
+      <c r="O2" s="97"/>
+      <c r="P2" s="97"/>
+      <c r="Q2" s="97"/>
+      <c r="R2" s="97"/>
+      <c r="S2" s="97"/>
+      <c r="T2" s="97"/>
+      <c r="U2" s="97"/>
+      <c r="V2" s="97"/>
+      <c r="W2" s="97"/>
+      <c r="X2" s="97"/>
+      <c r="Y2" s="97"/>
+      <c r="Z2" s="97"/>
+      <c r="AA2" s="97"/>
+      <c r="AB2" s="97"/>
+      <c r="AC2" s="97"/>
+      <c r="AD2" s="97"/>
+      <c r="AE2" s="97"/>
+      <c r="AF2" s="97"/>
+      <c r="AG2" s="97"/>
+      <c r="AH2" s="97"/>
     </row>
     <row r="3" spans="2:34" ht="12" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
@@ -2282,122 +2369,122 @@
     </row>
     <row r="4" spans="2:34" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="2:34" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="114" t="s">
+      <c r="B5" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="114"/>
-      <c r="D5" s="114"/>
-      <c r="E5" s="114"/>
-      <c r="F5" s="114"/>
-      <c r="G5" s="114"/>
-      <c r="H5" s="114"/>
-      <c r="I5" s="114"/>
-      <c r="J5" s="114"/>
-      <c r="L5" s="115" t="s">
+      <c r="C5" s="98"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="98"/>
+      <c r="F5" s="98"/>
+      <c r="G5" s="98"/>
+      <c r="H5" s="98"/>
+      <c r="I5" s="98"/>
+      <c r="J5" s="98"/>
+      <c r="L5" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="115"/>
-      <c r="N5" s="115"/>
-      <c r="O5" s="115"/>
-      <c r="P5" s="115"/>
-      <c r="R5" s="116" t="s">
+      <c r="M5" s="99"/>
+      <c r="N5" s="99"/>
+      <c r="O5" s="99"/>
+      <c r="P5" s="99"/>
+      <c r="R5" s="103" t="s">
         <v>11</v>
       </c>
-      <c r="S5" s="116"/>
-      <c r="T5" s="116"/>
-      <c r="U5" s="116"/>
-      <c r="V5" s="116"/>
-      <c r="W5" s="116"/>
-      <c r="X5" s="116"/>
-      <c r="Y5" s="116"/>
-      <c r="Z5" s="116"/>
-      <c r="AA5" s="116"/>
-      <c r="AB5" s="116"/>
-      <c r="AC5" s="116"/>
-      <c r="AD5" s="116"/>
-      <c r="AE5" s="116"/>
-      <c r="AF5" s="116"/>
-      <c r="AG5" s="116"/>
-      <c r="AH5" s="116"/>
+      <c r="S5" s="103"/>
+      <c r="T5" s="103"/>
+      <c r="U5" s="103"/>
+      <c r="V5" s="103"/>
+      <c r="W5" s="103"/>
+      <c r="X5" s="103"/>
+      <c r="Y5" s="103"/>
+      <c r="Z5" s="103"/>
+      <c r="AA5" s="103"/>
+      <c r="AB5" s="103"/>
+      <c r="AC5" s="103"/>
+      <c r="AD5" s="103"/>
+      <c r="AE5" s="103"/>
+      <c r="AF5" s="103"/>
+      <c r="AG5" s="103"/>
+      <c r="AH5" s="103"/>
     </row>
     <row r="6" spans="2:34" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="107" t="s">
+      <c r="B7" s="120" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="123" t="s">
+      <c r="C7" s="112" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="125" t="s">
+      <c r="D7" s="114" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="117" t="s">
+      <c r="E7" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="127" t="s">
+      <c r="F7" s="116" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="119" t="s">
+      <c r="G7" s="106" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="120"/>
-      <c r="I7" s="100" t="s">
+      <c r="H7" s="107"/>
+      <c r="I7" s="118" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="101"/>
+      <c r="J7" s="119"/>
       <c r="K7" s="4"/>
-      <c r="L7" s="121" t="s">
+      <c r="L7" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="M7" s="122"/>
-      <c r="N7" s="121" t="s">
-        <v>0</v>
-      </c>
-      <c r="O7" s="122"/>
-      <c r="P7" s="109" t="s">
+      <c r="M7" s="109"/>
+      <c r="N7" s="108" t="s">
+        <v>0</v>
+      </c>
+      <c r="O7" s="109"/>
+      <c r="P7" s="122" t="s">
         <v>42</v>
       </c>
       <c r="Q7" s="17"/>
-      <c r="R7" s="102" t="s">
+      <c r="R7" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="S7" s="103"/>
+      <c r="S7" s="111"/>
       <c r="T7" s="13"/>
-      <c r="U7" s="102" t="s">
+      <c r="U7" s="110" t="s">
         <v>38</v>
       </c>
-      <c r="V7" s="103"/>
-      <c r="W7" s="102" t="s">
+      <c r="V7" s="111"/>
+      <c r="W7" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="X7" s="103"/>
-      <c r="Y7" s="102" t="s">
+      <c r="X7" s="111"/>
+      <c r="Y7" s="110" t="s">
         <v>43</v>
       </c>
-      <c r="Z7" s="103"/>
-      <c r="AA7" s="102" t="s">
+      <c r="Z7" s="111"/>
+      <c r="AA7" s="110" t="s">
         <v>44</v>
       </c>
-      <c r="AB7" s="103"/>
-      <c r="AC7" s="102" t="s">
+      <c r="AB7" s="111"/>
+      <c r="AC7" s="110" t="s">
         <v>45</v>
       </c>
-      <c r="AD7" s="103"/>
-      <c r="AE7" s="102" t="s">
+      <c r="AD7" s="111"/>
+      <c r="AE7" s="110" t="s">
         <v>46</v>
       </c>
-      <c r="AF7" s="103"/>
+      <c r="AF7" s="111"/>
       <c r="AG7" s="13"/>
-      <c r="AH7" s="111" t="s">
+      <c r="AH7" s="124" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="2:34" ht="10.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="108"/>
-      <c r="C8" s="124"/>
-      <c r="D8" s="126"/>
-      <c r="E8" s="118"/>
-      <c r="F8" s="128"/>
+      <c r="B8" s="121"/>
+      <c r="C8" s="113"/>
+      <c r="D8" s="115"/>
+      <c r="E8" s="105"/>
+      <c r="F8" s="117"/>
       <c r="G8" s="18" t="s">
         <v>9</v>
       </c>
@@ -2423,7 +2510,7 @@
       <c r="O8" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="P8" s="110"/>
+      <c r="P8" s="123"/>
       <c r="Q8" s="17"/>
       <c r="R8" s="25" t="s">
         <v>9</v>
@@ -2469,7 +2556,7 @@
         <v>40</v>
       </c>
       <c r="AG8" s="16"/>
-      <c r="AH8" s="112"/>
+      <c r="AH8" s="125"/>
     </row>
     <row r="9" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="44" t="s">
@@ -4473,46 +4560,46 @@
       <c r="AH28" s="5"/>
     </row>
     <row r="29" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B29" s="104" t="s">
+      <c r="B29" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="105"/>
-      <c r="D29" s="106"/>
-      <c r="E29" s="104" t="s">
+      <c r="C29" s="101"/>
+      <c r="D29" s="102"/>
+      <c r="E29" s="100" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="106"/>
-      <c r="G29" s="104" t="s">
+      <c r="F29" s="102"/>
+      <c r="G29" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="H29" s="105"/>
-      <c r="I29" s="105"/>
-      <c r="J29" s="105"/>
-      <c r="K29" s="105"/>
-      <c r="L29" s="105"/>
-      <c r="M29" s="105"/>
-      <c r="N29" s="105"/>
-      <c r="O29" s="105"/>
-      <c r="P29" s="106"/>
-      <c r="R29" s="104" t="s">
+      <c r="H29" s="101"/>
+      <c r="I29" s="101"/>
+      <c r="J29" s="101"/>
+      <c r="K29" s="101"/>
+      <c r="L29" s="101"/>
+      <c r="M29" s="101"/>
+      <c r="N29" s="101"/>
+      <c r="O29" s="101"/>
+      <c r="P29" s="102"/>
+      <c r="R29" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="S29" s="105"/>
-      <c r="T29" s="105"/>
-      <c r="U29" s="105"/>
-      <c r="V29" s="105"/>
-      <c r="W29" s="105"/>
-      <c r="X29" s="105"/>
-      <c r="Y29" s="105"/>
-      <c r="Z29" s="105"/>
-      <c r="AA29" s="105"/>
-      <c r="AB29" s="105"/>
-      <c r="AC29" s="105"/>
-      <c r="AD29" s="105"/>
-      <c r="AE29" s="105"/>
-      <c r="AF29" s="105"/>
-      <c r="AG29" s="105"/>
-      <c r="AH29" s="106"/>
+      <c r="S29" s="101"/>
+      <c r="T29" s="101"/>
+      <c r="U29" s="101"/>
+      <c r="V29" s="101"/>
+      <c r="W29" s="101"/>
+      <c r="X29" s="101"/>
+      <c r="Y29" s="101"/>
+      <c r="Z29" s="101"/>
+      <c r="AA29" s="101"/>
+      <c r="AB29" s="101"/>
+      <c r="AC29" s="101"/>
+      <c r="AD29" s="101"/>
+      <c r="AE29" s="101"/>
+      <c r="AF29" s="101"/>
+      <c r="AG29" s="101"/>
+      <c r="AH29" s="102"/>
     </row>
     <row r="31" spans="2:34" x14ac:dyDescent="0.2">
       <c r="E31" s="10"/>
@@ -4891,6 +4978,16 @@
     <sortCondition ref="AL9"/>
   </sortState>
   <mergeCells count="26">
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="W7:X7"/>
+    <mergeCell ref="R29:AH29"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="Y7:Z7"/>
+    <mergeCell ref="AA7:AB7"/>
+    <mergeCell ref="AC7:AD7"/>
+    <mergeCell ref="AE7:AF7"/>
+    <mergeCell ref="AH7:AH8"/>
     <mergeCell ref="B2:AH2"/>
     <mergeCell ref="B5:J5"/>
     <mergeCell ref="L5:P5"/>
@@ -4907,16 +5004,6 @@
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="U7:V7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="W7:X7"/>
-    <mergeCell ref="R29:AH29"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="Y7:Z7"/>
-    <mergeCell ref="AA7:AB7"/>
-    <mergeCell ref="AC7:AD7"/>
-    <mergeCell ref="AE7:AF7"/>
-    <mergeCell ref="AH7:AH8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="125" orientation="portrait" r:id="rId1"/>
@@ -4929,15 +5016,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:AH33"/>
+  <dimension ref="A1:AX55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="N41" sqref="N41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="92"/>
+    <col min="1" max="1" width="10.6640625" style="149"/>
     <col min="2" max="2" width="31.5" style="92" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" style="92"/>
     <col min="4" max="4" width="16.6640625" style="92" bestFit="1" customWidth="1"/>
@@ -4948,917 +5035,1590 @@
     <col min="11" max="16384" width="10.6640625" style="92"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:34" ht="20.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="94" t="s">
+    <row r="1" spans="2:50" s="149" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:50" s="149" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="150" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
-      <c r="O2" s="95"/>
-      <c r="P2" s="95"/>
-      <c r="Q2" s="95"/>
-      <c r="R2" s="95"/>
-      <c r="S2" s="95"/>
-      <c r="T2" s="95"/>
-      <c r="U2" s="95"/>
-      <c r="V2" s="95"/>
-      <c r="W2" s="95"/>
-      <c r="X2" s="95"/>
-      <c r="Y2" s="95"/>
-      <c r="Z2" s="95"/>
-      <c r="AA2" s="95"/>
-      <c r="AB2" s="95"/>
-      <c r="AC2" s="95"/>
-      <c r="AD2" s="95"/>
-      <c r="AE2" s="95"/>
-      <c r="AF2" s="95"/>
-      <c r="AG2" s="95"/>
-      <c r="AH2" s="95"/>
-    </row>
-    <row r="3" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="96" t="s">
+      <c r="C2" s="151"/>
+      <c r="D2" s="151"/>
+      <c r="E2" s="151"/>
+      <c r="F2" s="151"/>
+      <c r="G2" s="151"/>
+      <c r="H2" s="151"/>
+      <c r="I2" s="151"/>
+      <c r="J2" s="151"/>
+      <c r="K2" s="151"/>
+      <c r="L2" s="151"/>
+      <c r="M2" s="151"/>
+      <c r="N2" s="151"/>
+      <c r="O2" s="151"/>
+      <c r="P2" s="151"/>
+      <c r="Q2" s="151"/>
+      <c r="R2" s="151"/>
+      <c r="S2" s="151"/>
+      <c r="T2" s="151"/>
+      <c r="U2" s="151"/>
+      <c r="V2" s="151"/>
+      <c r="W2" s="151"/>
+      <c r="X2" s="151"/>
+      <c r="Y2" s="151"/>
+      <c r="Z2" s="151"/>
+      <c r="AA2" s="151"/>
+      <c r="AB2" s="151"/>
+      <c r="AC2" s="151"/>
+      <c r="AD2" s="151"/>
+      <c r="AE2" s="151"/>
+      <c r="AF2" s="151"/>
+      <c r="AG2" s="151"/>
+      <c r="AH2" s="151"/>
+    </row>
+    <row r="3" spans="2:50" s="149" customFormat="1" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="152" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="129" t="s">
+    <row r="4" spans="2:50" s="149" customFormat="1" ht="10.35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="2:50" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="129"/>
-      <c r="D5" s="129"/>
-      <c r="E5" s="129"/>
-      <c r="F5" s="129"/>
-      <c r="G5" s="129"/>
-      <c r="H5" s="129"/>
-      <c r="I5" s="129"/>
-      <c r="J5" s="129"/>
-      <c r="L5" s="130" t="s">
+      <c r="C5" s="126"/>
+      <c r="D5" s="126"/>
+      <c r="E5" s="126"/>
+      <c r="F5" s="126"/>
+      <c r="G5" s="126"/>
+      <c r="H5" s="126"/>
+      <c r="I5" s="126"/>
+      <c r="J5" s="126"/>
+      <c r="L5" s="127" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="130"/>
-      <c r="N5" s="130"/>
-      <c r="O5" s="130"/>
-      <c r="P5" s="130"/>
-      <c r="R5" s="131" t="s">
+      <c r="M5" s="127"/>
+      <c r="N5" s="127"/>
+      <c r="O5" s="127"/>
+      <c r="P5" s="127"/>
+      <c r="R5" s="128" t="s">
         <v>11</v>
       </c>
-      <c r="S5" s="131"/>
-      <c r="T5" s="131"/>
-      <c r="U5" s="131"/>
-      <c r="V5" s="131"/>
-      <c r="W5" s="131"/>
-      <c r="X5" s="131"/>
-      <c r="Y5" s="131"/>
-      <c r="Z5" s="131"/>
-      <c r="AA5" s="131"/>
-      <c r="AB5" s="131"/>
-      <c r="AC5" s="131"/>
-      <c r="AD5" s="131"/>
-      <c r="AE5" s="131"/>
-      <c r="AF5" s="131"/>
-      <c r="AG5" s="131"/>
-      <c r="AH5" s="131"/>
-    </row>
-    <row r="6" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="132" t="s">
+      <c r="S5" s="128"/>
+      <c r="T5" s="128"/>
+      <c r="U5" s="128"/>
+      <c r="V5" s="128"/>
+      <c r="W5" s="128"/>
+      <c r="X5" s="128"/>
+      <c r="Y5" s="128"/>
+      <c r="Z5" s="128"/>
+      <c r="AA5" s="128"/>
+      <c r="AB5" s="128"/>
+      <c r="AC5" s="128"/>
+      <c r="AD5" s="128"/>
+      <c r="AE5" s="128"/>
+      <c r="AF5" s="128"/>
+      <c r="AG5" s="128"/>
+      <c r="AH5" s="128"/>
+    </row>
+    <row r="6" spans="2:50" s="149" customFormat="1" ht="10.35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="2:50" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="142" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="132" t="s">
+      <c r="C7" s="142" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="132" t="s">
+      <c r="D7" s="129" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="133" t="s">
+      <c r="E7" s="130" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="133" t="s">
+      <c r="F7" s="143" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="132" t="s">
+      <c r="G7" s="141" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="132"/>
-      <c r="I7" s="132" t="s">
+      <c r="H7" s="144"/>
+      <c r="I7" s="141" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="132"/>
-      <c r="L7" s="92" t="s">
+      <c r="J7" s="144"/>
+      <c r="K7" s="149"/>
+      <c r="L7" s="149" t="s">
         <v>2</v>
       </c>
-      <c r="N7" s="92" t="s">
-        <v>0</v>
-      </c>
-      <c r="P7" s="93" t="s">
+      <c r="M7" s="149"/>
+      <c r="N7" s="149" t="s">
+        <v>0</v>
+      </c>
+      <c r="O7" s="149"/>
+      <c r="P7" s="153" t="s">
         <v>42</v>
       </c>
-      <c r="R7" s="92" t="s">
+      <c r="Q7" s="149"/>
+      <c r="R7" s="149" t="s">
         <v>5</v>
       </c>
-      <c r="U7" s="92" t="s">
+      <c r="S7" s="149"/>
+      <c r="T7" s="149"/>
+      <c r="U7" s="149" t="s">
         <v>38</v>
       </c>
-      <c r="W7" s="92" t="s">
+      <c r="V7" s="149"/>
+      <c r="W7" s="149" t="s">
         <v>41</v>
       </c>
-      <c r="Y7" s="92" t="s">
+      <c r="X7" s="149"/>
+      <c r="Y7" s="149" t="s">
         <v>43</v>
       </c>
-      <c r="AA7" s="92" t="s">
+      <c r="Z7" s="149"/>
+      <c r="AA7" s="149" t="s">
         <v>44</v>
       </c>
-      <c r="AC7" s="92" t="s">
+      <c r="AB7" s="149"/>
+      <c r="AC7" s="149" t="s">
         <v>45</v>
       </c>
-      <c r="AE7" s="92" t="s">
+      <c r="AD7" s="149"/>
+      <c r="AE7" s="149" t="s">
         <v>46</v>
       </c>
-      <c r="AH7" s="93" t="s">
+      <c r="AF7" s="149"/>
+      <c r="AG7" s="149"/>
+      <c r="AH7" s="153" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="132"/>
-      <c r="C8" s="132"/>
-      <c r="D8" s="132"/>
-      <c r="E8" s="133"/>
-      <c r="F8" s="133"/>
-      <c r="G8" s="97" t="s">
+      <c r="AI7" s="149"/>
+      <c r="AJ7" s="149"/>
+      <c r="AK7" s="149"/>
+      <c r="AL7" s="149"/>
+      <c r="AM7" s="149"/>
+      <c r="AN7" s="149"/>
+      <c r="AO7" s="149"/>
+      <c r="AP7" s="149"/>
+      <c r="AQ7" s="149"/>
+      <c r="AR7" s="149"/>
+      <c r="AS7" s="149"/>
+      <c r="AT7" s="149"/>
+      <c r="AU7" s="149"/>
+      <c r="AV7" s="149"/>
+      <c r="AW7" s="149"/>
+      <c r="AX7" s="149"/>
+    </row>
+    <row r="8" spans="2:50" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="142"/>
+      <c r="C8" s="142"/>
+      <c r="D8" s="129"/>
+      <c r="E8" s="130"/>
+      <c r="F8" s="143"/>
+      <c r="G8" s="145" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="97" t="s">
+      <c r="H8" s="146" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="97" t="s">
+      <c r="I8" s="145" t="s">
         <v>3</v>
       </c>
-      <c r="J8" s="97" t="s">
+      <c r="J8" s="146" t="s">
         <v>4</v>
       </c>
-      <c r="L8" s="92" t="s">
+      <c r="K8" s="149"/>
+      <c r="L8" s="149" t="s">
         <v>9</v>
       </c>
-      <c r="M8" s="92" t="s">
+      <c r="M8" s="149" t="s">
         <v>8</v>
       </c>
-      <c r="N8" s="92" t="s">
+      <c r="N8" s="149" t="s">
         <v>3</v>
       </c>
-      <c r="O8" s="92" t="s">
+      <c r="O8" s="149" t="s">
         <v>4</v>
       </c>
-      <c r="P8" s="93"/>
-      <c r="AH8" s="93"/>
-    </row>
-    <row r="9" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="93" t="s">
+      <c r="P8" s="153"/>
+      <c r="Q8" s="149"/>
+      <c r="R8" s="149"/>
+      <c r="S8" s="149"/>
+      <c r="T8" s="149"/>
+      <c r="U8" s="149"/>
+      <c r="V8" s="149"/>
+      <c r="W8" s="149"/>
+      <c r="X8" s="149"/>
+      <c r="Y8" s="149"/>
+      <c r="Z8" s="149"/>
+      <c r="AA8" s="149"/>
+      <c r="AB8" s="149"/>
+      <c r="AC8" s="149"/>
+      <c r="AD8" s="149"/>
+      <c r="AE8" s="149"/>
+      <c r="AF8" s="149"/>
+      <c r="AG8" s="149"/>
+      <c r="AH8" s="153"/>
+      <c r="AI8" s="149"/>
+      <c r="AJ8" s="149"/>
+      <c r="AK8" s="149"/>
+      <c r="AL8" s="149"/>
+      <c r="AM8" s="149"/>
+      <c r="AN8" s="149"/>
+      <c r="AO8" s="149"/>
+      <c r="AP8" s="149"/>
+      <c r="AQ8" s="149"/>
+      <c r="AR8" s="149"/>
+      <c r="AS8" s="149"/>
+      <c r="AT8" s="149"/>
+      <c r="AU8" s="149"/>
+      <c r="AV8" s="149"/>
+      <c r="AW8" s="149"/>
+      <c r="AX8" s="149"/>
+    </row>
+    <row r="9" spans="2:50" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="136" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="93" t="s">
+      <c r="C9" s="136" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="98">
+      <c r="D9" s="93">
         <v>38226</v>
       </c>
-      <c r="E9" s="99" t="s">
+      <c r="E9" s="94" t="s">
         <v>69</v>
       </c>
-      <c r="G9" s="92">
+      <c r="F9" s="139"/>
+      <c r="G9" s="147">
         <v>21.68</v>
       </c>
-      <c r="H9" s="92">
+      <c r="H9" s="139">
         <v>32.520000000000003</v>
       </c>
-      <c r="I9" s="92">
+      <c r="I9" s="147">
         <v>86639.77</v>
       </c>
-      <c r="J9" s="92">
+      <c r="J9" s="139">
         <v>138605.66</v>
       </c>
-      <c r="K9" s="92">
-        <v>0</v>
-      </c>
-      <c r="L9" s="92">
+      <c r="K9" s="149">
+        <v>0</v>
+      </c>
+      <c r="L9" s="149">
         <v>1837.5</v>
       </c>
-      <c r="M9" s="92">
+      <c r="M9" s="149">
         <v>12.7</v>
       </c>
-      <c r="N9" s="92">
+      <c r="N9" s="149">
         <v>87225.33</v>
       </c>
-      <c r="O9" s="92">
+      <c r="O9" s="149">
         <v>113521.61</v>
       </c>
-      <c r="P9" s="92">
+      <c r="P9" s="149">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="138" t="s">
+      <c r="Q9" s="149"/>
+      <c r="R9" s="149"/>
+      <c r="S9" s="149"/>
+      <c r="T9" s="149"/>
+      <c r="U9" s="149"/>
+      <c r="V9" s="149"/>
+      <c r="W9" s="149"/>
+      <c r="X9" s="149"/>
+      <c r="Y9" s="149"/>
+      <c r="Z9" s="149"/>
+      <c r="AA9" s="149"/>
+      <c r="AB9" s="149"/>
+      <c r="AC9" s="149"/>
+      <c r="AD9" s="149"/>
+      <c r="AE9" s="149"/>
+      <c r="AF9" s="149"/>
+      <c r="AG9" s="149"/>
+      <c r="AH9" s="149"/>
+      <c r="AI9" s="149"/>
+      <c r="AJ9" s="149"/>
+      <c r="AK9" s="149"/>
+      <c r="AL9" s="149"/>
+      <c r="AM9" s="149"/>
+      <c r="AN9" s="149"/>
+      <c r="AO9" s="149"/>
+      <c r="AP9" s="149"/>
+      <c r="AQ9" s="149"/>
+      <c r="AR9" s="149"/>
+      <c r="AS9" s="149"/>
+      <c r="AT9" s="149"/>
+      <c r="AU9" s="149"/>
+      <c r="AV9" s="149"/>
+      <c r="AW9" s="149"/>
+      <c r="AX9" s="149"/>
+    </row>
+    <row r="10" spans="2:50" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="135" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="138" t="s">
+      <c r="C10" s="135" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="139">
+      <c r="D10" s="95">
         <v>37601</v>
       </c>
-      <c r="E10" s="140"/>
-      <c r="F10" s="140"/>
-      <c r="G10" s="140">
+      <c r="E10" s="96"/>
+      <c r="F10" s="138"/>
+      <c r="G10" s="148">
         <v>23.05</v>
       </c>
-      <c r="H10" s="140">
+      <c r="H10" s="138">
         <v>34.58</v>
       </c>
-      <c r="I10" s="140">
+      <c r="I10" s="148">
         <v>86104.49</v>
       </c>
-      <c r="J10" s="140">
+      <c r="J10" s="138">
         <v>141119.44</v>
       </c>
-      <c r="K10" s="92">
-        <v>0</v>
-      </c>
-      <c r="L10" s="92">
+      <c r="K10" s="149">
+        <v>0</v>
+      </c>
+      <c r="L10" s="149">
         <v>1800</v>
       </c>
-      <c r="M10" s="92">
+      <c r="M10" s="149">
         <v>25.2</v>
       </c>
-      <c r="N10" s="92">
+      <c r="N10" s="149">
         <v>100494.47</v>
       </c>
-      <c r="O10" s="92">
+      <c r="O10" s="149">
         <v>133202.71</v>
       </c>
-      <c r="P10" s="92">
+      <c r="P10" s="149">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="93" t="s">
+      <c r="Q10" s="149"/>
+      <c r="R10" s="149"/>
+      <c r="S10" s="149"/>
+      <c r="T10" s="149"/>
+      <c r="U10" s="149"/>
+      <c r="V10" s="149"/>
+      <c r="W10" s="149"/>
+      <c r="X10" s="149"/>
+      <c r="Y10" s="149"/>
+      <c r="Z10" s="149"/>
+      <c r="AA10" s="149"/>
+      <c r="AB10" s="149"/>
+      <c r="AC10" s="149"/>
+      <c r="AD10" s="149"/>
+      <c r="AE10" s="149"/>
+      <c r="AF10" s="149"/>
+      <c r="AG10" s="149"/>
+      <c r="AH10" s="149"/>
+      <c r="AI10" s="149"/>
+      <c r="AJ10" s="149"/>
+      <c r="AK10" s="149"/>
+      <c r="AL10" s="149"/>
+      <c r="AM10" s="149"/>
+      <c r="AN10" s="149"/>
+      <c r="AO10" s="149"/>
+      <c r="AP10" s="149"/>
+      <c r="AQ10" s="149"/>
+      <c r="AR10" s="149"/>
+      <c r="AS10" s="149"/>
+      <c r="AT10" s="149"/>
+      <c r="AU10" s="149"/>
+      <c r="AV10" s="149"/>
+      <c r="AW10" s="149"/>
+      <c r="AX10" s="149"/>
+    </row>
+    <row r="11" spans="2:50" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="136" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="93" t="s">
+      <c r="C11" s="136" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="98">
+      <c r="D11" s="93">
         <v>35826</v>
       </c>
-      <c r="G11" s="92">
+      <c r="F11" s="139"/>
+      <c r="G11" s="147">
         <v>26.94</v>
       </c>
-      <c r="H11" s="92">
+      <c r="H11" s="139">
         <v>40.409999999999997</v>
       </c>
-      <c r="I11" s="92">
+      <c r="I11" s="147">
         <v>89605.86</v>
       </c>
-      <c r="J11" s="92">
+      <c r="J11" s="139">
         <v>156292.04</v>
       </c>
-      <c r="K11" s="92">
-        <v>0</v>
-      </c>
-      <c r="L11" s="92">
+      <c r="K11" s="149">
+        <v>0</v>
+      </c>
+      <c r="L11" s="149">
         <v>1800</v>
       </c>
-      <c r="M11" s="92">
-        <v>0</v>
-      </c>
-      <c r="N11" s="92">
+      <c r="M11" s="149">
+        <v>0</v>
+      </c>
+      <c r="N11" s="149">
         <v>76821.77</v>
       </c>
-      <c r="O11" s="92">
+      <c r="O11" s="149">
         <v>158727.13</v>
       </c>
-      <c r="P11" s="92">
+      <c r="P11" s="149">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="138" t="s">
+      <c r="Q11" s="149"/>
+      <c r="R11" s="149"/>
+      <c r="S11" s="149"/>
+      <c r="T11" s="149"/>
+      <c r="U11" s="149"/>
+      <c r="V11" s="149"/>
+      <c r="W11" s="149"/>
+      <c r="X11" s="149"/>
+      <c r="Y11" s="149"/>
+      <c r="Z11" s="149"/>
+      <c r="AA11" s="149"/>
+      <c r="AB11" s="149"/>
+      <c r="AC11" s="149"/>
+      <c r="AD11" s="149"/>
+      <c r="AE11" s="149"/>
+      <c r="AF11" s="149"/>
+      <c r="AG11" s="149"/>
+      <c r="AH11" s="149"/>
+      <c r="AI11" s="149"/>
+      <c r="AJ11" s="149"/>
+      <c r="AK11" s="149"/>
+      <c r="AL11" s="149"/>
+      <c r="AM11" s="149"/>
+      <c r="AN11" s="149"/>
+      <c r="AO11" s="149"/>
+      <c r="AP11" s="149"/>
+      <c r="AQ11" s="149"/>
+      <c r="AR11" s="149"/>
+      <c r="AS11" s="149"/>
+      <c r="AT11" s="149"/>
+      <c r="AU11" s="149"/>
+      <c r="AV11" s="149"/>
+      <c r="AW11" s="149"/>
+      <c r="AX11" s="149"/>
+    </row>
+    <row r="12" spans="2:50" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="135" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="138" t="s">
+      <c r="C12" s="135" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="139">
+      <c r="D12" s="95">
         <v>35403</v>
       </c>
-      <c r="E12" s="140"/>
-      <c r="F12" s="140"/>
-      <c r="G12" s="140">
+      <c r="E12" s="96"/>
+      <c r="F12" s="138"/>
+      <c r="G12" s="148">
         <v>27.87</v>
       </c>
-      <c r="H12" s="140">
+      <c r="H12" s="138">
         <v>41.81</v>
       </c>
-      <c r="I12" s="140">
+      <c r="I12" s="148">
         <v>88556.09</v>
       </c>
-      <c r="J12" s="140">
+      <c r="J12" s="138">
         <v>156576.41</v>
       </c>
-      <c r="K12" s="92">
-        <v>0</v>
-      </c>
-      <c r="L12" s="92">
+      <c r="K12" s="149">
+        <v>0</v>
+      </c>
+      <c r="L12" s="149">
         <v>1762.5</v>
       </c>
-      <c r="M12" s="92">
-        <v>0</v>
-      </c>
-      <c r="N12" s="92">
+      <c r="M12" s="149">
+        <v>0</v>
+      </c>
+      <c r="N12" s="149">
         <v>77813.539999999994</v>
       </c>
-      <c r="O12" s="92">
+      <c r="O12" s="149">
         <v>170576.59</v>
       </c>
-      <c r="P12" s="92">
+      <c r="P12" s="149">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="93" t="s">
+      <c r="Q12" s="149"/>
+      <c r="R12" s="149"/>
+      <c r="S12" s="149"/>
+      <c r="T12" s="149"/>
+      <c r="U12" s="149"/>
+      <c r="V12" s="149"/>
+      <c r="W12" s="149"/>
+      <c r="X12" s="149"/>
+      <c r="Y12" s="149"/>
+      <c r="Z12" s="149"/>
+      <c r="AA12" s="149"/>
+      <c r="AB12" s="149"/>
+      <c r="AC12" s="149"/>
+      <c r="AD12" s="149"/>
+      <c r="AE12" s="149"/>
+      <c r="AF12" s="149"/>
+      <c r="AG12" s="149"/>
+      <c r="AH12" s="149"/>
+      <c r="AI12" s="149"/>
+      <c r="AJ12" s="149"/>
+      <c r="AK12" s="149"/>
+      <c r="AL12" s="149"/>
+      <c r="AM12" s="149"/>
+      <c r="AN12" s="149"/>
+      <c r="AO12" s="149"/>
+      <c r="AP12" s="149"/>
+      <c r="AQ12" s="149"/>
+      <c r="AR12" s="149"/>
+      <c r="AS12" s="149"/>
+      <c r="AT12" s="149"/>
+      <c r="AU12" s="149"/>
+      <c r="AV12" s="149"/>
+      <c r="AW12" s="149"/>
+      <c r="AX12" s="149"/>
+    </row>
+    <row r="13" spans="2:50" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="136" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="93" t="s">
+      <c r="C13" s="136" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="98">
+      <c r="D13" s="93">
         <v>33093</v>
       </c>
-      <c r="G13" s="92">
+      <c r="F13" s="139"/>
+      <c r="G13" s="147">
         <v>32.93</v>
       </c>
-      <c r="H13" s="92">
+      <c r="H13" s="139">
         <v>49.4</v>
       </c>
-      <c r="I13" s="92">
+      <c r="I13" s="147">
         <v>91038.77</v>
       </c>
-      <c r="J13" s="92">
+      <c r="J13" s="139">
         <v>172168.01</v>
       </c>
-      <c r="K13" s="92">
-        <v>0</v>
-      </c>
-      <c r="L13" s="92">
+      <c r="K13" s="149">
+        <v>0</v>
+      </c>
+      <c r="L13" s="149">
         <v>1725</v>
       </c>
-      <c r="M13" s="92">
+      <c r="M13" s="149">
         <v>39.57</v>
       </c>
-      <c r="N13" s="92">
+      <c r="N13" s="149">
         <v>96236.12</v>
       </c>
-      <c r="O13" s="92">
+      <c r="O13" s="149">
         <v>177509.88</v>
       </c>
-      <c r="P13" s="92">
+      <c r="P13" s="149">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="138" t="s">
+      <c r="Q13" s="149"/>
+      <c r="R13" s="149"/>
+      <c r="S13" s="149"/>
+      <c r="T13" s="149"/>
+      <c r="U13" s="149"/>
+      <c r="V13" s="149"/>
+      <c r="W13" s="149"/>
+      <c r="X13" s="149"/>
+      <c r="Y13" s="149"/>
+      <c r="Z13" s="149"/>
+      <c r="AA13" s="149"/>
+      <c r="AB13" s="149"/>
+      <c r="AC13" s="149"/>
+      <c r="AD13" s="149"/>
+      <c r="AE13" s="149"/>
+      <c r="AF13" s="149"/>
+      <c r="AG13" s="149"/>
+      <c r="AH13" s="149"/>
+      <c r="AI13" s="149"/>
+      <c r="AJ13" s="149"/>
+      <c r="AK13" s="149"/>
+      <c r="AL13" s="149"/>
+      <c r="AM13" s="149"/>
+      <c r="AN13" s="149"/>
+      <c r="AO13" s="149"/>
+      <c r="AP13" s="149"/>
+      <c r="AQ13" s="149"/>
+      <c r="AR13" s="149"/>
+      <c r="AS13" s="149"/>
+      <c r="AT13" s="149"/>
+      <c r="AU13" s="149"/>
+      <c r="AV13" s="149"/>
+      <c r="AW13" s="149"/>
+      <c r="AX13" s="149"/>
+    </row>
+    <row r="14" spans="2:50" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="135" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="138" t="s">
+      <c r="C14" s="135" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="139">
+      <c r="D14" s="95">
         <v>37900</v>
       </c>
-      <c r="E14" s="140"/>
-      <c r="F14" s="140"/>
-      <c r="G14" s="140">
+      <c r="E14" s="96"/>
+      <c r="F14" s="138"/>
+      <c r="G14" s="148">
         <v>22.4</v>
       </c>
-      <c r="H14" s="140">
+      <c r="H14" s="138">
         <v>33.6</v>
       </c>
-      <c r="I14" s="140">
+      <c r="I14" s="148">
         <v>87296.23</v>
       </c>
-      <c r="J14" s="140">
+      <c r="J14" s="138">
         <v>141450.34</v>
       </c>
-      <c r="K14" s="92">
-        <v>0</v>
-      </c>
-      <c r="L14" s="92">
+      <c r="K14" s="149">
+        <v>0</v>
+      </c>
+      <c r="L14" s="149">
         <v>1837.5</v>
       </c>
-      <c r="M14" s="92">
+      <c r="M14" s="149">
         <v>98.2</v>
       </c>
-      <c r="N14" s="92">
+      <c r="N14" s="149">
         <v>86363.33</v>
       </c>
-      <c r="O14" s="92">
+      <c r="O14" s="149">
         <v>120584.13</v>
       </c>
-      <c r="P14" s="92">
+      <c r="P14" s="149">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="93" t="s">
+      <c r="Q14" s="149"/>
+      <c r="R14" s="149"/>
+      <c r="S14" s="149"/>
+      <c r="T14" s="149"/>
+      <c r="U14" s="149"/>
+      <c r="V14" s="149"/>
+      <c r="W14" s="149"/>
+      <c r="X14" s="149"/>
+      <c r="Y14" s="149"/>
+      <c r="Z14" s="149"/>
+      <c r="AA14" s="149"/>
+      <c r="AB14" s="149"/>
+      <c r="AC14" s="149"/>
+      <c r="AD14" s="149"/>
+      <c r="AE14" s="149"/>
+      <c r="AF14" s="149"/>
+      <c r="AG14" s="149"/>
+      <c r="AH14" s="149"/>
+      <c r="AI14" s="149"/>
+      <c r="AJ14" s="149"/>
+      <c r="AK14" s="149"/>
+      <c r="AL14" s="149"/>
+      <c r="AM14" s="149"/>
+      <c r="AN14" s="149"/>
+      <c r="AO14" s="149"/>
+      <c r="AP14" s="149"/>
+      <c r="AQ14" s="149"/>
+      <c r="AR14" s="149"/>
+      <c r="AS14" s="149"/>
+      <c r="AT14" s="149"/>
+      <c r="AU14" s="149"/>
+      <c r="AV14" s="149"/>
+      <c r="AW14" s="149"/>
+      <c r="AX14" s="149"/>
+    </row>
+    <row r="15" spans="2:50" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="136" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="93" t="s">
+      <c r="C15" s="136" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="98">
+      <c r="D15" s="93">
         <v>35590</v>
       </c>
-      <c r="G15" s="92">
+      <c r="F15" s="139"/>
+      <c r="G15" s="147">
         <v>27.46</v>
       </c>
-      <c r="H15" s="92">
+      <c r="H15" s="139">
         <v>41.19</v>
       </c>
-      <c r="I15" s="92">
+      <c r="I15" s="147">
         <v>88194.9</v>
       </c>
-      <c r="J15" s="92">
+      <c r="J15" s="139">
         <v>155011.24</v>
       </c>
-      <c r="K15" s="92">
-        <v>0</v>
-      </c>
-      <c r="L15" s="92">
+      <c r="K15" s="149">
+        <v>0</v>
+      </c>
+      <c r="L15" s="149">
         <v>1762.5</v>
       </c>
-      <c r="M15" s="92">
+      <c r="M15" s="149">
         <v>244.14</v>
       </c>
-      <c r="N15" s="92">
+      <c r="N15" s="149">
         <v>98812.43</v>
       </c>
-      <c r="O15" s="92">
+      <c r="O15" s="149">
         <v>119521.7</v>
       </c>
-      <c r="P15" s="92">
+      <c r="P15" s="149">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="2:34" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="138" t="s">
+      <c r="Q15" s="149"/>
+      <c r="R15" s="149"/>
+      <c r="S15" s="149"/>
+      <c r="T15" s="149"/>
+      <c r="U15" s="149"/>
+      <c r="V15" s="149"/>
+      <c r="W15" s="149"/>
+      <c r="X15" s="149"/>
+      <c r="Y15" s="149"/>
+      <c r="Z15" s="149"/>
+      <c r="AA15" s="149"/>
+      <c r="AB15" s="149"/>
+      <c r="AC15" s="149"/>
+      <c r="AD15" s="149"/>
+      <c r="AE15" s="149"/>
+      <c r="AF15" s="149"/>
+      <c r="AG15" s="149"/>
+      <c r="AH15" s="149"/>
+      <c r="AI15" s="149"/>
+      <c r="AJ15" s="149"/>
+      <c r="AK15" s="149"/>
+      <c r="AL15" s="149"/>
+      <c r="AM15" s="149"/>
+      <c r="AN15" s="149"/>
+      <c r="AO15" s="149"/>
+      <c r="AP15" s="149"/>
+      <c r="AQ15" s="149"/>
+      <c r="AR15" s="149"/>
+      <c r="AS15" s="149"/>
+      <c r="AT15" s="149"/>
+      <c r="AU15" s="149"/>
+      <c r="AV15" s="149"/>
+      <c r="AW15" s="149"/>
+      <c r="AX15" s="149"/>
+    </row>
+    <row r="16" spans="2:50" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="135" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="138" t="s">
+      <c r="C16" s="135" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="139">
+      <c r="D16" s="95">
         <v>35192</v>
       </c>
-      <c r="E16" s="140"/>
-      <c r="F16" s="140"/>
-      <c r="G16" s="140">
+      <c r="E16" s="96"/>
+      <c r="F16" s="138"/>
+      <c r="G16" s="148">
         <v>28.33</v>
       </c>
-      <c r="H16" s="140">
+      <c r="H16" s="138">
         <v>42.5</v>
       </c>
-      <c r="I16" s="140">
+      <c r="I16" s="148">
         <v>88963.64</v>
       </c>
-      <c r="J16" s="140">
+      <c r="J16" s="138">
         <v>158342.45000000001</v>
       </c>
-      <c r="K16" s="92">
-        <v>0</v>
-      </c>
-      <c r="L16" s="92">
+      <c r="K16" s="149">
+        <v>0</v>
+      </c>
+      <c r="L16" s="149">
         <v>1762.5</v>
       </c>
-      <c r="M16" s="92">
+      <c r="M16" s="149">
         <v>109.39</v>
       </c>
-      <c r="N16" s="92">
+      <c r="N16" s="149">
         <v>89879.18</v>
       </c>
-      <c r="O16" s="92">
+      <c r="O16" s="149">
         <v>164850.17000000001</v>
       </c>
-      <c r="P16" s="92">
+      <c r="P16" s="149">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="2:18" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="93" t="s">
+      <c r="Q16" s="149"/>
+      <c r="R16" s="149"/>
+      <c r="S16" s="149"/>
+      <c r="T16" s="149"/>
+      <c r="U16" s="149"/>
+      <c r="V16" s="149"/>
+      <c r="W16" s="149"/>
+      <c r="X16" s="149"/>
+      <c r="Y16" s="149"/>
+      <c r="Z16" s="149"/>
+      <c r="AA16" s="149"/>
+      <c r="AB16" s="149"/>
+      <c r="AC16" s="149"/>
+      <c r="AD16" s="149"/>
+      <c r="AE16" s="149"/>
+      <c r="AF16" s="149"/>
+      <c r="AG16" s="149"/>
+      <c r="AH16" s="149"/>
+      <c r="AI16" s="149"/>
+      <c r="AJ16" s="149"/>
+      <c r="AK16" s="149"/>
+      <c r="AL16" s="149"/>
+      <c r="AM16" s="149"/>
+      <c r="AN16" s="149"/>
+      <c r="AO16" s="149"/>
+      <c r="AP16" s="149"/>
+      <c r="AQ16" s="149"/>
+      <c r="AR16" s="149"/>
+      <c r="AS16" s="149"/>
+      <c r="AT16" s="149"/>
+      <c r="AU16" s="149"/>
+      <c r="AV16" s="149"/>
+      <c r="AW16" s="149"/>
+      <c r="AX16" s="149"/>
+    </row>
+    <row r="17" spans="2:50" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="136" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="93" t="s">
+      <c r="C17" s="136" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="98">
+      <c r="D17" s="93">
         <v>36628</v>
       </c>
-      <c r="G17" s="92">
+      <c r="F17" s="139"/>
+      <c r="G17" s="147">
         <v>25.19</v>
       </c>
-      <c r="H17" s="92">
+      <c r="H17" s="139">
         <v>37.78</v>
       </c>
-      <c r="I17" s="92">
+      <c r="I17" s="147">
         <v>88023.83</v>
       </c>
-      <c r="J17" s="92">
+      <c r="J17" s="139">
         <v>149436.59</v>
       </c>
-      <c r="K17" s="92">
-        <v>0</v>
-      </c>
-      <c r="L17" s="92">
+      <c r="K17" s="149">
+        <v>0</v>
+      </c>
+      <c r="L17" s="149">
         <v>1800</v>
       </c>
-      <c r="M17" s="92">
-        <v>0</v>
-      </c>
-      <c r="N17" s="92">
+      <c r="M17" s="149">
+        <v>0</v>
+      </c>
+      <c r="N17" s="149">
         <v>92616.29</v>
       </c>
-      <c r="O17" s="92">
+      <c r="O17" s="149">
         <v>149766.94</v>
       </c>
-      <c r="P17" s="92">
+      <c r="P17" s="149">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="2:18" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="138" t="s">
+      <c r="Q17" s="149"/>
+      <c r="R17" s="149"/>
+      <c r="S17" s="149"/>
+      <c r="T17" s="149"/>
+      <c r="U17" s="149"/>
+      <c r="V17" s="149"/>
+      <c r="W17" s="149"/>
+      <c r="X17" s="149"/>
+      <c r="Y17" s="149"/>
+      <c r="Z17" s="149"/>
+      <c r="AA17" s="149"/>
+      <c r="AB17" s="149"/>
+      <c r="AC17" s="149"/>
+      <c r="AD17" s="149"/>
+      <c r="AE17" s="149"/>
+      <c r="AF17" s="149"/>
+      <c r="AG17" s="149"/>
+      <c r="AH17" s="149"/>
+      <c r="AI17" s="149"/>
+      <c r="AJ17" s="149"/>
+      <c r="AK17" s="149"/>
+      <c r="AL17" s="149"/>
+      <c r="AM17" s="149"/>
+      <c r="AN17" s="149"/>
+      <c r="AO17" s="149"/>
+      <c r="AP17" s="149"/>
+      <c r="AQ17" s="149"/>
+      <c r="AR17" s="149"/>
+      <c r="AS17" s="149"/>
+      <c r="AT17" s="149"/>
+      <c r="AU17" s="149"/>
+      <c r="AV17" s="149"/>
+      <c r="AW17" s="149"/>
+      <c r="AX17" s="149"/>
+    </row>
+    <row r="18" spans="2:50" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="135" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="138" t="s">
+      <c r="C18" s="135" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="139">
+      <c r="D18" s="95">
         <v>30115</v>
       </c>
-      <c r="E18" s="140"/>
-      <c r="F18" s="140"/>
-      <c r="G18" s="140">
+      <c r="E18" s="96"/>
+      <c r="F18" s="138"/>
+      <c r="G18" s="148">
         <v>39.46</v>
       </c>
-      <c r="H18" s="140">
+      <c r="H18" s="138">
         <v>59.19</v>
       </c>
-      <c r="I18" s="140">
+      <c r="I18" s="148">
         <v>92465.44</v>
       </c>
-      <c r="J18" s="140">
+      <c r="J18" s="138">
         <v>188016.91</v>
       </c>
-      <c r="K18" s="92">
-        <v>0</v>
-      </c>
-      <c r="L18" s="92">
+      <c r="K18" s="149">
+        <v>0</v>
+      </c>
+      <c r="L18" s="149">
         <v>1650</v>
       </c>
-      <c r="M18" s="92">
+      <c r="M18" s="149">
         <v>143.27000000000001</v>
       </c>
-      <c r="N18" s="92">
+      <c r="N18" s="149">
         <v>86538.68</v>
       </c>
-      <c r="O18" s="92">
+      <c r="O18" s="149">
         <v>168507.1</v>
       </c>
-      <c r="P18" s="92">
+      <c r="P18" s="149">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="2:18" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="93" t="s">
+      <c r="Q18" s="149"/>
+      <c r="R18" s="149"/>
+      <c r="S18" s="149"/>
+      <c r="T18" s="149"/>
+      <c r="U18" s="149"/>
+      <c r="V18" s="149"/>
+      <c r="W18" s="149"/>
+      <c r="X18" s="149"/>
+      <c r="Y18" s="149"/>
+      <c r="Z18" s="149"/>
+      <c r="AA18" s="149"/>
+      <c r="AB18" s="149"/>
+      <c r="AC18" s="149"/>
+      <c r="AD18" s="149"/>
+      <c r="AE18" s="149"/>
+      <c r="AF18" s="149"/>
+      <c r="AG18" s="149"/>
+      <c r="AH18" s="149"/>
+      <c r="AI18" s="149"/>
+      <c r="AJ18" s="149"/>
+      <c r="AK18" s="149"/>
+      <c r="AL18" s="149"/>
+      <c r="AM18" s="149"/>
+      <c r="AN18" s="149"/>
+      <c r="AO18" s="149"/>
+      <c r="AP18" s="149"/>
+      <c r="AQ18" s="149"/>
+      <c r="AR18" s="149"/>
+      <c r="AS18" s="149"/>
+      <c r="AT18" s="149"/>
+      <c r="AU18" s="149"/>
+      <c r="AV18" s="149"/>
+      <c r="AW18" s="149"/>
+      <c r="AX18" s="149"/>
+    </row>
+    <row r="19" spans="2:50" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="136" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="93" t="s">
+      <c r="C19" s="136" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="98">
+      <c r="D19" s="93">
         <v>41231</v>
       </c>
-      <c r="G19" s="92">
+      <c r="F19" s="139"/>
+      <c r="G19" s="147">
         <v>15.1</v>
       </c>
-      <c r="H19" s="92">
+      <c r="H19" s="139">
         <v>22.64</v>
       </c>
-      <c r="I19" s="92">
+      <c r="I19" s="147">
         <v>82233.27</v>
       </c>
-      <c r="J19" s="92">
+      <c r="J19" s="139">
         <v>114677.5</v>
       </c>
-      <c r="K19" s="92">
-        <v>0</v>
-      </c>
-      <c r="L19" s="92">
+      <c r="K19" s="149">
+        <v>0</v>
+      </c>
+      <c r="L19" s="149">
         <v>1875</v>
       </c>
-      <c r="M19" s="92">
-        <v>0</v>
-      </c>
-      <c r="N19" s="92">
+      <c r="M19" s="149">
+        <v>0</v>
+      </c>
+      <c r="N19" s="149">
         <v>74240.86</v>
       </c>
-      <c r="O19" s="92">
+      <c r="O19" s="149">
         <v>112740.09</v>
       </c>
-      <c r="P19" s="92">
+      <c r="P19" s="149">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="2:18" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="138" t="s">
+      <c r="Q19" s="149"/>
+      <c r="R19" s="149"/>
+      <c r="S19" s="149"/>
+      <c r="T19" s="149"/>
+      <c r="U19" s="149"/>
+      <c r="V19" s="149"/>
+      <c r="W19" s="149"/>
+      <c r="X19" s="149"/>
+      <c r="Y19" s="149"/>
+      <c r="Z19" s="149"/>
+      <c r="AA19" s="149"/>
+      <c r="AB19" s="149"/>
+      <c r="AC19" s="149"/>
+      <c r="AD19" s="149"/>
+      <c r="AE19" s="149"/>
+      <c r="AF19" s="149"/>
+      <c r="AG19" s="149"/>
+      <c r="AH19" s="149"/>
+      <c r="AI19" s="149"/>
+      <c r="AJ19" s="149"/>
+      <c r="AK19" s="149"/>
+      <c r="AL19" s="149"/>
+      <c r="AM19" s="149"/>
+      <c r="AN19" s="149"/>
+      <c r="AO19" s="149"/>
+      <c r="AP19" s="149"/>
+      <c r="AQ19" s="149"/>
+      <c r="AR19" s="149"/>
+      <c r="AS19" s="149"/>
+      <c r="AT19" s="149"/>
+      <c r="AU19" s="149"/>
+      <c r="AV19" s="149"/>
+      <c r="AW19" s="149"/>
+      <c r="AX19" s="149"/>
+    </row>
+    <row r="20" spans="2:50" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="135" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="138" t="s">
+      <c r="C20" s="135" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="139">
+      <c r="D20" s="95">
         <v>31824</v>
       </c>
-      <c r="E20" s="140"/>
-      <c r="F20" s="140"/>
-      <c r="G20" s="140">
+      <c r="E20" s="96"/>
+      <c r="F20" s="138"/>
+      <c r="G20" s="148">
         <v>35.71</v>
       </c>
-      <c r="H20" s="140">
+      <c r="H20" s="138">
         <v>53.57</v>
       </c>
-      <c r="I20" s="140">
+      <c r="I20" s="148">
         <v>91406.45</v>
       </c>
-      <c r="J20" s="140">
+      <c r="J20" s="138">
         <v>178594.61</v>
       </c>
-      <c r="K20" s="92">
-        <v>0</v>
-      </c>
-      <c r="L20" s="92">
+      <c r="K20" s="149">
+        <v>0</v>
+      </c>
+      <c r="L20" s="149">
         <v>1687.5</v>
       </c>
-      <c r="M20" s="92">
+      <c r="M20" s="149">
         <v>145.13</v>
       </c>
-      <c r="N20" s="92">
+      <c r="N20" s="149">
         <v>90744.11</v>
       </c>
-      <c r="O20" s="92">
+      <c r="O20" s="149">
         <v>180217.79</v>
       </c>
-      <c r="P20" s="92">
+      <c r="P20" s="149">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="2:18" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="93" t="s">
+      <c r="Q20" s="149"/>
+      <c r="R20" s="149"/>
+      <c r="S20" s="149"/>
+      <c r="T20" s="149"/>
+      <c r="U20" s="149"/>
+      <c r="V20" s="149"/>
+      <c r="W20" s="149"/>
+      <c r="X20" s="149"/>
+      <c r="Y20" s="149"/>
+      <c r="Z20" s="149"/>
+      <c r="AA20" s="149"/>
+      <c r="AB20" s="149"/>
+      <c r="AC20" s="149"/>
+      <c r="AD20" s="149"/>
+      <c r="AE20" s="149"/>
+      <c r="AF20" s="149"/>
+      <c r="AG20" s="149"/>
+      <c r="AH20" s="149"/>
+      <c r="AI20" s="149"/>
+      <c r="AJ20" s="149"/>
+      <c r="AK20" s="149"/>
+      <c r="AL20" s="149"/>
+      <c r="AM20" s="149"/>
+      <c r="AN20" s="149"/>
+      <c r="AO20" s="149"/>
+      <c r="AP20" s="149"/>
+      <c r="AQ20" s="149"/>
+      <c r="AR20" s="149"/>
+      <c r="AS20" s="149"/>
+      <c r="AT20" s="149"/>
+      <c r="AU20" s="149"/>
+      <c r="AV20" s="149"/>
+      <c r="AW20" s="149"/>
+      <c r="AX20" s="149"/>
+    </row>
+    <row r="21" spans="2:50" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="136" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="93" t="s">
+      <c r="C21" s="136" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="98">
+      <c r="D21" s="93">
         <v>38150</v>
       </c>
-      <c r="G21" s="92">
+      <c r="F21" s="139"/>
+      <c r="G21" s="147">
         <v>21.85</v>
       </c>
-      <c r="H21" s="92">
+      <c r="H21" s="139">
         <v>32.770000000000003</v>
       </c>
-      <c r="I21" s="92">
+      <c r="I21" s="147">
         <v>86792.81</v>
       </c>
-      <c r="J21" s="92">
+      <c r="J21" s="139">
         <v>139268.84</v>
       </c>
-      <c r="K21" s="92">
-        <v>0</v>
-      </c>
-      <c r="L21" s="92">
+      <c r="K21" s="149">
+        <v>0</v>
+      </c>
+      <c r="L21" s="149">
         <v>1837.5</v>
       </c>
-      <c r="M21" s="92">
+      <c r="M21" s="149">
         <v>191.85</v>
       </c>
-      <c r="N21" s="92">
+      <c r="N21" s="149">
         <v>92277.83</v>
       </c>
-      <c r="O21" s="92">
+      <c r="O21" s="149">
         <v>139124.15</v>
       </c>
-      <c r="P21" s="92">
+      <c r="P21" s="149">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="2:18" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="138" t="s">
+      <c r="Q21" s="149"/>
+      <c r="R21" s="149"/>
+      <c r="S21" s="149"/>
+      <c r="T21" s="149"/>
+      <c r="U21" s="149"/>
+      <c r="V21" s="149"/>
+      <c r="W21" s="149"/>
+      <c r="X21" s="149"/>
+      <c r="Y21" s="149"/>
+      <c r="Z21" s="149"/>
+      <c r="AA21" s="149"/>
+      <c r="AB21" s="149"/>
+      <c r="AC21" s="149"/>
+      <c r="AD21" s="149"/>
+      <c r="AE21" s="149"/>
+      <c r="AF21" s="149"/>
+      <c r="AG21" s="149"/>
+      <c r="AH21" s="149"/>
+      <c r="AI21" s="149"/>
+      <c r="AJ21" s="149"/>
+      <c r="AK21" s="149"/>
+      <c r="AL21" s="149"/>
+      <c r="AM21" s="149"/>
+      <c r="AN21" s="149"/>
+      <c r="AO21" s="149"/>
+      <c r="AP21" s="149"/>
+      <c r="AQ21" s="149"/>
+      <c r="AR21" s="149"/>
+      <c r="AS21" s="149"/>
+      <c r="AT21" s="149"/>
+      <c r="AU21" s="149"/>
+      <c r="AV21" s="149"/>
+      <c r="AW21" s="149"/>
+      <c r="AX21" s="149"/>
+    </row>
+    <row r="22" spans="2:50" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="135" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="138" t="s">
+      <c r="C22" s="135" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="139">
+      <c r="D22" s="95">
         <v>32891</v>
       </c>
-      <c r="E22" s="140"/>
-      <c r="F22" s="140"/>
-      <c r="G22" s="140">
+      <c r="E22" s="96"/>
+      <c r="F22" s="138"/>
+      <c r="G22" s="148">
         <v>33.380000000000003</v>
       </c>
-      <c r="H22" s="140">
+      <c r="H22" s="138">
         <v>50.06</v>
       </c>
-      <c r="I22" s="140">
+      <c r="I22" s="148">
         <v>91420.63</v>
       </c>
-      <c r="J22" s="140">
+      <c r="J22" s="138">
         <v>173822.75</v>
       </c>
-      <c r="K22" s="92">
-        <v>0</v>
-      </c>
-      <c r="L22" s="92">
+      <c r="K22" s="149">
+        <v>0</v>
+      </c>
+      <c r="L22" s="149">
         <v>1725</v>
       </c>
-      <c r="M22" s="92">
+      <c r="M22" s="149">
         <v>150.72</v>
       </c>
-      <c r="N22" s="92">
+      <c r="N22" s="149">
         <v>80527.14</v>
       </c>
-      <c r="O22" s="92">
+      <c r="O22" s="149">
         <v>181545.58</v>
       </c>
-      <c r="P22" s="92">
+      <c r="P22" s="149">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="2:18" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="93" t="s">
+      <c r="Q22" s="149"/>
+      <c r="R22" s="149"/>
+      <c r="S22" s="149"/>
+      <c r="T22" s="149"/>
+      <c r="U22" s="149"/>
+      <c r="V22" s="149"/>
+      <c r="W22" s="149"/>
+      <c r="X22" s="149"/>
+      <c r="Y22" s="149"/>
+      <c r="Z22" s="149"/>
+      <c r="AA22" s="149"/>
+      <c r="AB22" s="149"/>
+      <c r="AC22" s="149"/>
+      <c r="AD22" s="149"/>
+      <c r="AE22" s="149"/>
+      <c r="AF22" s="149"/>
+      <c r="AG22" s="149"/>
+      <c r="AH22" s="149"/>
+      <c r="AI22" s="149"/>
+      <c r="AJ22" s="149"/>
+      <c r="AK22" s="149"/>
+      <c r="AL22" s="149"/>
+      <c r="AM22" s="149"/>
+      <c r="AN22" s="149"/>
+      <c r="AO22" s="149"/>
+      <c r="AP22" s="149"/>
+      <c r="AQ22" s="149"/>
+      <c r="AR22" s="149"/>
+      <c r="AS22" s="149"/>
+      <c r="AT22" s="149"/>
+      <c r="AU22" s="149"/>
+      <c r="AV22" s="149"/>
+      <c r="AW22" s="149"/>
+      <c r="AX22" s="149"/>
+    </row>
+    <row r="23" spans="2:50" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="136" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="93" t="s">
+      <c r="C23" s="136" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="98">
+      <c r="D23" s="93">
         <v>41102</v>
       </c>
-      <c r="G23" s="92">
+      <c r="F23" s="139"/>
+      <c r="G23" s="147">
         <v>15.38</v>
       </c>
-      <c r="H23" s="92">
+      <c r="H23" s="139">
         <v>23.07</v>
       </c>
-      <c r="I23" s="92">
+      <c r="I23" s="147">
         <v>82498.34</v>
       </c>
-      <c r="J23" s="92">
+      <c r="J23" s="139">
         <v>115826.13</v>
       </c>
-      <c r="K23" s="92">
-        <v>0</v>
-      </c>
-      <c r="L23" s="92">
+      <c r="K23" s="149">
+        <v>0</v>
+      </c>
+      <c r="L23" s="149">
         <v>1875</v>
       </c>
-      <c r="M23" s="92">
+      <c r="M23" s="149">
         <v>159.16999999999999</v>
       </c>
-      <c r="N23" s="92">
+      <c r="N23" s="149">
         <v>73878.58</v>
       </c>
-      <c r="O23" s="92">
+      <c r="O23" s="149">
         <v>125469.62</v>
       </c>
-      <c r="P23" s="92">
+      <c r="P23" s="149">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="2:18" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="140" t="s">
+      <c r="Q23" s="149"/>
+      <c r="R23" s="149"/>
+      <c r="S23" s="149"/>
+      <c r="T23" s="149"/>
+      <c r="U23" s="149"/>
+      <c r="V23" s="149"/>
+      <c r="W23" s="149"/>
+      <c r="X23" s="149"/>
+      <c r="Y23" s="149"/>
+      <c r="Z23" s="149"/>
+      <c r="AA23" s="149"/>
+      <c r="AB23" s="149"/>
+      <c r="AC23" s="149"/>
+      <c r="AD23" s="149"/>
+      <c r="AE23" s="149"/>
+      <c r="AF23" s="149"/>
+      <c r="AG23" s="149"/>
+      <c r="AH23" s="149"/>
+      <c r="AI23" s="149"/>
+      <c r="AJ23" s="149"/>
+      <c r="AK23" s="149"/>
+      <c r="AL23" s="149"/>
+      <c r="AM23" s="149"/>
+      <c r="AN23" s="149"/>
+      <c r="AO23" s="149"/>
+      <c r="AP23" s="149"/>
+      <c r="AQ23" s="149"/>
+      <c r="AR23" s="149"/>
+      <c r="AS23" s="149"/>
+      <c r="AT23" s="149"/>
+      <c r="AU23" s="149"/>
+      <c r="AV23" s="149"/>
+      <c r="AW23" s="149"/>
+      <c r="AX23" s="149"/>
+    </row>
+    <row r="24" spans="2:50" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="137" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="140" t="s">
+      <c r="C24" s="137" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="139">
+      <c r="D24" s="95">
         <v>29465</v>
       </c>
-      <c r="E24" s="140"/>
-      <c r="F24" s="140"/>
-      <c r="G24" s="140">
+      <c r="E24" s="96"/>
+      <c r="F24" s="138"/>
+      <c r="G24" s="148">
         <v>40.880000000000003</v>
       </c>
-      <c r="H24" s="140">
+      <c r="H24" s="138">
         <v>61.33</v>
       </c>
-      <c r="I24" s="140">
+      <c r="I24" s="148">
         <v>93640.78</v>
       </c>
-      <c r="J24" s="140">
+      <c r="J24" s="138">
         <v>193110.06</v>
       </c>
-      <c r="K24" s="92">
-        <v>0</v>
-      </c>
-      <c r="L24" s="92">
+      <c r="K24" s="149">
+        <v>0</v>
+      </c>
+      <c r="L24" s="149">
         <v>1650</v>
       </c>
-      <c r="M24" s="92">
-        <v>0</v>
-      </c>
-      <c r="N24" s="92">
+      <c r="M24" s="149">
+        <v>0</v>
+      </c>
+      <c r="N24" s="149">
         <v>83732.44</v>
       </c>
-      <c r="O24" s="92">
+      <c r="O24" s="149">
         <v>208951.82</v>
       </c>
-      <c r="P24" s="92">
+      <c r="P24" s="149">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="2:18" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="92" t="s">
+      <c r="Q24" s="149"/>
+      <c r="R24" s="149"/>
+      <c r="S24" s="149"/>
+      <c r="T24" s="149"/>
+      <c r="U24" s="149"/>
+      <c r="V24" s="149"/>
+      <c r="W24" s="149"/>
+      <c r="X24" s="149"/>
+      <c r="Y24" s="149"/>
+      <c r="Z24" s="149"/>
+      <c r="AA24" s="149"/>
+      <c r="AB24" s="149"/>
+      <c r="AC24" s="149"/>
+      <c r="AD24" s="149"/>
+      <c r="AE24" s="149"/>
+      <c r="AF24" s="149"/>
+      <c r="AG24" s="149"/>
+      <c r="AH24" s="149"/>
+      <c r="AI24" s="149"/>
+      <c r="AJ24" s="149"/>
+      <c r="AK24" s="149"/>
+      <c r="AL24" s="149"/>
+      <c r="AM24" s="149"/>
+      <c r="AN24" s="149"/>
+      <c r="AO24" s="149"/>
+      <c r="AP24" s="149"/>
+      <c r="AQ24" s="149"/>
+      <c r="AR24" s="149"/>
+      <c r="AS24" s="149"/>
+      <c r="AT24" s="149"/>
+      <c r="AU24" s="149"/>
+      <c r="AV24" s="149"/>
+      <c r="AW24" s="149"/>
+      <c r="AX24" s="149"/>
+    </row>
+    <row r="25" spans="2:50" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="140" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="92" t="s">
+      <c r="C25" s="140" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="98">
+      <c r="D25" s="93">
         <v>30711</v>
       </c>
-      <c r="G25" s="92">
+      <c r="F25" s="139"/>
+      <c r="G25" s="147">
         <v>38.15</v>
       </c>
-      <c r="H25" s="92">
+      <c r="H25" s="139">
         <v>57.23</v>
       </c>
-      <c r="I25" s="92">
+      <c r="I25" s="147">
         <v>93464.74</v>
       </c>
-      <c r="J25" s="92">
+      <c r="J25" s="139">
         <v>187513.86</v>
       </c>
-      <c r="K25" s="92">
-        <v>0</v>
-      </c>
-      <c r="L25" s="92">
+      <c r="K25" s="149">
+        <v>0</v>
+      </c>
+      <c r="L25" s="149">
         <v>1687.5</v>
       </c>
-      <c r="M25" s="92">
+      <c r="M25" s="149">
         <v>226.41</v>
       </c>
-      <c r="N25" s="92">
+      <c r="N25" s="149">
         <v>98278.63</v>
       </c>
-      <c r="O25" s="92">
+      <c r="O25" s="149">
         <v>171337.91</v>
       </c>
-      <c r="P25" s="92">
+      <c r="P25" s="149">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="2:18" ht="10.35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="2:18" ht="10.35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="2:18" ht="10.35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B29" s="92" t="s">
+      <c r="Q25" s="149"/>
+      <c r="R25" s="149"/>
+      <c r="S25" s="149"/>
+      <c r="T25" s="149"/>
+      <c r="U25" s="149"/>
+      <c r="V25" s="149"/>
+      <c r="W25" s="149"/>
+      <c r="X25" s="149"/>
+      <c r="Y25" s="149"/>
+      <c r="Z25" s="149"/>
+      <c r="AA25" s="149"/>
+      <c r="AB25" s="149"/>
+      <c r="AC25" s="149"/>
+      <c r="AD25" s="149"/>
+      <c r="AE25" s="149"/>
+      <c r="AF25" s="149"/>
+      <c r="AG25" s="149"/>
+      <c r="AH25" s="149"/>
+      <c r="AI25" s="149"/>
+      <c r="AJ25" s="149"/>
+      <c r="AK25" s="149"/>
+      <c r="AL25" s="149"/>
+      <c r="AM25" s="149"/>
+      <c r="AN25" s="149"/>
+      <c r="AO25" s="149"/>
+      <c r="AP25" s="149"/>
+      <c r="AQ25" s="149"/>
+      <c r="AR25" s="149"/>
+      <c r="AS25" s="149"/>
+      <c r="AT25" s="149"/>
+      <c r="AU25" s="149"/>
+      <c r="AV25" s="149"/>
+      <c r="AW25" s="149"/>
+      <c r="AX25" s="149"/>
+    </row>
+    <row r="26" spans="2:50" s="149" customFormat="1" ht="10.35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="2:50" s="149" customFormat="1" ht="10.35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="2:50" s="149" customFormat="1" ht="10.35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="2:50" s="149" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="149" t="s">
         <v>12</v>
       </c>
-      <c r="E29" s="92" t="s">
+      <c r="E29" s="149" t="s">
         <v>49</v>
       </c>
-      <c r="G29" s="92" t="s">
+      <c r="G29" s="149" t="s">
         <v>12</v>
       </c>
-      <c r="R29" s="92" t="s">
+      <c r="R29" s="149" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="2:18" ht="10.35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="2:18" ht="10.35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="2:18" ht="10.35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="10.35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="2:50" s="149" customFormat="1" ht="10.35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="2:50" s="149" customFormat="1" ht="10.35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="2:50" s="149" customFormat="1" ht="10.35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="149" customFormat="1" ht="10.35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="149" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="149" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="149" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="149" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="149" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="149" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="149" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="149" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="149" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="149" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="149" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="149" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="149" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="149" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="149" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="149" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="149" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="149" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="149" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="149" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="149" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="55" s="149" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="B5:J5"/>
@@ -5897,15 +6657,15 @@
   <sheetData>
     <row r="1" spans="2:4" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B2" s="134" t="s">
+      <c r="B2" s="131" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="134"/>
-      <c r="D2" s="134"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
     </row>
     <row r="3" spans="2:4" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C4" s="135" t="s">
+      <c r="C4" s="132" t="s">
         <v>59</v>
       </c>
       <c r="D4" s="88" t="s">
@@ -5913,25 +6673,25 @@
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C5" s="136"/>
+      <c r="C5" s="133"/>
       <c r="D5" s="70" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C6" s="136"/>
+      <c r="C6" s="133"/>
       <c r="D6" s="71" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C7" s="136"/>
+      <c r="C7" s="133"/>
       <c r="D7" s="70" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="137"/>
+      <c r="C8" s="134"/>
       <c r="D8" s="89" t="s">
         <v>56</v>
       </c>
@@ -5951,7 +6711,7 @@
       <c r="C11" s="72"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C12" s="135" t="s">
+      <c r="C12" s="132" t="s">
         <v>57</v>
       </c>
       <c r="D12" s="88" t="s">
@@ -5959,43 +6719,43 @@
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C13" s="136"/>
+      <c r="C13" s="133"/>
       <c r="D13" s="70" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C14" s="136"/>
+      <c r="C14" s="133"/>
       <c r="D14" s="68" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C15" s="136"/>
+      <c r="C15" s="133"/>
       <c r="D15" s="87" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C16" s="136"/>
+      <c r="C16" s="133"/>
       <c r="D16" s="68" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C17" s="136"/>
+      <c r="C17" s="133"/>
       <c r="D17" s="87" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C18" s="136"/>
+      <c r="C18" s="133"/>
       <c r="D18" s="68" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="19" spans="3:4" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="137"/>
+      <c r="C19" s="134"/>
       <c r="D19" s="89" t="s">
         <v>61</v>
       </c>

</xml_diff>